<commit_message>
Add properties of Maven Compiler Plugin
</commit_message>
<xml_diff>
--- a/arrays.xlsx
+++ b/arrays.xlsx
@@ -6,10 +6,10 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sorted Array(Min to Max) + 1" r:id="rId3" sheetId="1"/>
+    <sheet name="Sorted Array(Max to Min)" r:id="rId3" sheetId="1"/>
     <sheet name="Sorted Array(Min to Max)" r:id="rId4" sheetId="2"/>
-    <sheet name="Random Array" r:id="rId5" sheetId="3"/>
-    <sheet name="Sorted Array(Max to Min)" r:id="rId6" sheetId="4"/>
+    <sheet name="Sorted Array(Min to Max) + 1" r:id="rId5" sheetId="3"/>
+    <sheet name="Random Array" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
@@ -23,10 +23,10 @@
     <t>Bubble Sort (Up)</t>
   </si>
   <si>
-    <t>Bubble Sort (Down)</t>
+    <t>Selection Sort</t>
   </si>
   <si>
-    <t>Selection Sort</t>
+    <t>Bubble Sort (Down)</t>
   </si>
   <si>
     <t>Native Sort</t>
@@ -84,7 +84,7 @@
           <a:bodyPr/>
           <a:p>
             <a:r>
-              <a:t>Sorted Array(Min to Max) + 1</a:t>
+              <a:t>Sorted Array(Max to Min)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -105,64 +105,64 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>501.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1501.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2501.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3501.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4501.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5501.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6501.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7501.0</c:v>
+              <c:f>'Sorted Array(Max to Min)'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$2:$I$2</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>4090820.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5217364.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1937947.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5399688.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7826046.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.9846799E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.5221687E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.1258905E7</c:v>
+              <c:f>'Sorted Array(Max to Min)'!$B$2:$I$2</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6381340.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6735120.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6200827.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0935214E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.810924E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.9148897E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9139237E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2597357E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -171,6 +171,80 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Selection Sort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sorted Array(Max to Min)'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sorted Array(Max to Min)'!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3604823.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6997740.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7776541.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1333066E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7640752E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1690059E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.273742E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0819444E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Bubble Sort (Down)</c:v>
           </c:tx>
@@ -179,138 +253,64 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>501.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1501.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2501.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3501.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4501.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5501.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6501.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7501.0</c:v>
+              <c:f>'Sorted Array(Max to Min)'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$3:$I$3</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>5067641.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1971755.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7367218.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9782105.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.6805201E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.9507508E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.8572391E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.909647E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Selection Sort</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>501.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1501.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2501.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3501.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4501.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5501.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6501.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7501.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$4:$I$4</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>3422499.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2681732.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4645035.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8202164.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.3426774E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.7718632E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.6273418E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.2196485E7</c:v>
+              <c:f>'Sorted Array(Max to Min)'!$B$4:$I$4</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6957894.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7379292.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4291303E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0004926E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4269666E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.7174365E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.6237944E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.6372067E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -327,64 +327,64 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>501.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1501.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2501.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3501.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4501.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5501.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6501.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7501.0</c:v>
+              <c:f>'Sorted Array(Max to Min)'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$5:$I$5</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>81503.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>165420.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>301258.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>136441.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>137045.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>264430.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>307898.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>357403.0</c:v>
+              <c:f>'Sorted Array(Max to Min)'!$B$5:$I$5</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>877812.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>225792.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>980444.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>516182.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>664094.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>207680.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>213114.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>307295.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -401,64 +401,64 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>501.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1501.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2501.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3501.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4501.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5501.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6501.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7501.0</c:v>
+              <c:f>'Sorted Array(Max to Min)'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$6:$I$6</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1409087.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1546736.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2373834.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2468015.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2940125.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1614352.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1574506.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2003149.0</c:v>
+              <c:f>'Sorted Array(Max to Min)'!$B$6:$I$6</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1840748.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500852.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3885554.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2699240.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4249598.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1705515.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1633671.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1994093.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -613,28 +613,28 @@
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>126782.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1208047.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7303826.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6081290.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6873977.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9742862.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.2829088E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.0793991E7</c:v>
+                  <c:v>516182.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1485760.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3587315.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5858565E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1130215E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6051153E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.493673E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0281479E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -643,6 +643,80 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Selection Sort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sorted Array(Min to Max)'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sorted Array(Min to Max)'!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>236056.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2161928.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5903192.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8618129.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0515072E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4881791E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4312022E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.3035707E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Bubble Sort (Down)</c:v>
           </c:tx>
@@ -683,106 +757,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$3:$I$3</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>260204.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2054465.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6478539.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.6792522E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7396848E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.5691986E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.8642423E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.3470386E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Selection Sort</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>500.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1500.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3500.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5500.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6500.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7500.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
               <c:f>'Sorted Array(Min to Max)'!$B$4:$I$4</c:f>
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>182928.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1560018.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5524055.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8834865.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.3412284E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.7407111E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.660904E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.3303711E7</c:v>
+                  <c:v>257789.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2037561.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6484577.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9782105.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0806066E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.762631E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.5178919E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2182647E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -835,28 +835,28 @@
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>25960.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>58561.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>81503.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>36827.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22338.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>34412.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43468.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                  <c:v>22941.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45883.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>138253.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33205.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29582.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35016.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42864.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52523.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -909,28 +909,28 @@
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>123160.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>350762.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>575951.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>588629.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>709977.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1197180.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1654198.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1889649.0</c:v>
+                  <c:v>111689.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>420794.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>560254.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>534897.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>907394.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1345092.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1075833.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2110008.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1028,7 +1028,7 @@
           <a:bodyPr/>
           <a:p>
             <a:r>
-              <a:t>Random Array</a:t>
+              <a:t>Sorted Array(Min to Max) + 1</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1049,64 +1049,64 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Random Array'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>500.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1500.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3500.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5500.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6500.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7500.0</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>501.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1501.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2501.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3501.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4501.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5501.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6501.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7501.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Random Array'!$B$2:$I$2</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>388193.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2926240.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.8002985E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.2884679E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.1544465E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.0991553E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.7344058E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.06484334E8</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$2:$I$2</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>173268.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1267816.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3139353.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7723414.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0256027E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.593403E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5366773E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5798989E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1115,6 +1115,80 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Selection Sort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>501.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1501.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2501.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3501.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4501.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5501.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6501.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7501.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>255374.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1815392.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5282566.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1332462E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3574686E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3678574E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.8494704E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.697021E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Bubble Sort (Down)</c:v>
           </c:tx>
@@ -1123,138 +1197,64 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Random Array'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>500.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1500.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3500.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5500.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6500.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7500.0</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>501.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1501.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2501.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3501.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4501.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5501.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6501.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7501.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Random Array'!$B$3:$I$3</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>574743.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4326875.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.4014798E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.0932243E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0450014E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.4194346E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.06966829E8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.78788596E8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Selection Sort</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Random Array'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>500.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1500.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3500.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5500.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6500.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7500.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Random Array'!$B$4:$I$4</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>225188.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1595033.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4512217.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6502084.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0304324E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.562915E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.4183333E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.9322866E7</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$4:$I$4</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>255374.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2270598.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5560882.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1256394E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3747954E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0119126E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.9900628E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9078599E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1271,64 +1271,64 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Random Array'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>500.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1500.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3500.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5500.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6500.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7500.0</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>501.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1501.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2501.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3501.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4501.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5501.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6501.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7501.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Random Array'!$B$5:$I$5</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>36224.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64599.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>99011.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>111085.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>102029.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>123763.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>247526.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>211303.0</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$5:$I$5</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10264.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15093.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20527.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22941.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32601.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38638.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1887234.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65806.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1345,64 +1345,64 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Random Array'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>500.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1500.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3500.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5500.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6500.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7500.0</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>501.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1501.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2501.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3501.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4501.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5501.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6501.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7501.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Random Array'!$B$6:$I$6</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>127989.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>386382.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1297399.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>962937.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>839173.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1590203.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1801506.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2166758.0</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$6:$I$6</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>103236.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>302465.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>674358.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>868756.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1203218.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1345695.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1450743.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2476467.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1500,7 +1500,7 @@
           <a:bodyPr/>
           <a:p>
             <a:r>
-              <a:t>Sorted Array(Max to Min)</a:t>
+              <a:t>Random Array</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1521,7 +1521,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$1:$I$1</c:f>
+              <c:f>'Random Array'!$B$1:$I$1</c:f>
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1553,32 +1553,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$2:$I$2</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>307898.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3337374.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7883400.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.3613976E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.8520422E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.3894102E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.4925307E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.7742273E7</c:v>
+              <c:f>'Random Array'!$B$2:$I$2</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>396645.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5429875.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9495337.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1540795E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.936643E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5711449E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.9525257E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.1576753E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,6 +1587,80 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Selection Sort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Random Array'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3500.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5500.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Random Array'!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>239074.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1692836.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5853687.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.374735E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7386126E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.3333342E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.2420514E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0294761E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Bubble Sort (Down)</c:v>
           </c:tx>
@@ -1595,7 +1669,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$1:$I$1</c:f>
+              <c:f>'Random Array'!$B$1:$I$1</c:f>
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1627,106 +1701,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$3:$I$3</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>469092.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9057034.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.2393806E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.5669044E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.721648E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.9689325E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.5781626E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.046646E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Selection Sort</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>500.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1500.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3500.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5500.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6500.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7500.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$4:$I$4</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>199832.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2714333.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4349212.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8402600.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.6305923E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.7183227E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.7976469E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.8607359E7</c:v>
+              <c:f>'Random Array'!$B$4:$I$4</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>717825.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4488672.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7089554E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3644765E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.7821506E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.182423E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.5042115E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.06106526E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1743,7 +1743,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$1:$I$1</c:f>
+              <c:f>'Random Array'!$B$1:$I$1</c:f>
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1775,32 +1775,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$5:$I$5</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>13282.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21130.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26563.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>38035.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45279.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>144894.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>37431.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>71239.0</c:v>
+              <c:f>'Random Array'!$B$5:$I$5</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>38034.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63391.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82710.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>101426.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>136441.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>159986.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>193191.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>137649.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1817,7 +1817,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$1:$I$1</c:f>
+              <c:f>'Random Array'!$B$1:$I$1</c:f>
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1849,32 +1849,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$6:$I$6</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>115311.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>340499.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>901356.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>868152.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1042024.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2379268.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1226762.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1846785.0</c:v>
+              <c:f>'Random Array'!$B$6:$I$6</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>124971.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>382759.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>734729.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1051080.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250912.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1491193.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1723625.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1331207.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2119,28 +2119,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>501.0</v>
+        <v>500.0</v>
       </c>
       <c r="C1" t="n">
-        <v>1501.0</v>
+        <v>1500.0</v>
       </c>
       <c r="D1" t="n">
-        <v>2501.0</v>
+        <v>2500.0</v>
       </c>
       <c r="E1" t="n">
-        <v>3501.0</v>
+        <v>3500.0</v>
       </c>
       <c r="F1" t="n">
-        <v>4501.0</v>
+        <v>4500.0</v>
       </c>
       <c r="G1" t="n">
-        <v>5501.0</v>
+        <v>5500.0</v>
       </c>
       <c r="H1" t="n">
-        <v>6501.0</v>
+        <v>6500.0</v>
       </c>
       <c r="I1" t="n">
-        <v>7501.0</v>
+        <v>7500.0</v>
       </c>
     </row>
     <row r="2">
@@ -2148,28 +2148,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>4090820.0</v>
+        <v>6381340.0</v>
       </c>
       <c r="C2" t="n">
-        <v>5217364.0</v>
+        <v>6735120.0</v>
       </c>
       <c r="D2" t="n">
-        <v>1937947.0</v>
+        <v>6200827.0</v>
       </c>
       <c r="E2" t="n">
-        <v>5399688.0</v>
+        <v>1.0935214E7</v>
       </c>
       <c r="F2" t="n">
-        <v>7826046.0</v>
+        <v>1.810924E7</v>
       </c>
       <c r="G2" t="n">
-        <v>2.9846799E7</v>
+        <v>2.9148897E7</v>
       </c>
       <c r="H2" t="n">
-        <v>2.5221687E7</v>
+        <v>2.9139237E7</v>
       </c>
       <c r="I2" t="n">
-        <v>3.1258905E7</v>
+        <v>3.2597357E7</v>
       </c>
     </row>
     <row r="3">
@@ -2177,28 +2177,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>5067641.0</v>
+        <v>3604823.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1971755.0</v>
+        <v>6997740.0</v>
       </c>
       <c r="D3" t="n">
-        <v>7367218.0</v>
+        <v>7776541.0</v>
       </c>
       <c r="E3" t="n">
-        <v>9782105.0</v>
+        <v>1.1333066E7</v>
       </c>
       <c r="F3" t="n">
-        <v>1.6805201E7</v>
+        <v>1.7640752E7</v>
       </c>
       <c r="G3" t="n">
-        <v>2.9507508E7</v>
+        <v>5.1690059E7</v>
       </c>
       <c r="H3" t="n">
-        <v>3.8572391E7</v>
+        <v>3.273742E7</v>
       </c>
       <c r="I3" t="n">
-        <v>4.909647E7</v>
+        <v>4.0819444E7</v>
       </c>
     </row>
     <row r="4">
@@ -2206,28 +2206,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3422499.0</v>
+        <v>6957894.0</v>
       </c>
       <c r="C4" t="n">
-        <v>2681732.0</v>
+        <v>7379292.0</v>
       </c>
       <c r="D4" t="n">
-        <v>4645035.0</v>
+        <v>1.4291303E7</v>
       </c>
       <c r="E4" t="n">
-        <v>8202164.0</v>
+        <v>2.0004926E7</v>
       </c>
       <c r="F4" t="n">
-        <v>1.3426774E7</v>
+        <v>3.4269666E7</v>
       </c>
       <c r="G4" t="n">
-        <v>1.7718632E7</v>
+        <v>7.7174365E7</v>
       </c>
       <c r="H4" t="n">
-        <v>3.6273418E7</v>
+        <v>6.6237944E7</v>
       </c>
       <c r="I4" t="n">
-        <v>3.2196485E7</v>
+        <v>8.6372067E7</v>
       </c>
     </row>
     <row r="5">
@@ -2235,28 +2235,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>81503.0</v>
+        <v>877812.0</v>
       </c>
       <c r="C5" t="n">
-        <v>165420.0</v>
+        <v>225792.0</v>
       </c>
       <c r="D5" t="n">
-        <v>301258.0</v>
+        <v>980444.0</v>
       </c>
       <c r="E5" t="n">
-        <v>136441.0</v>
+        <v>516182.0</v>
       </c>
       <c r="F5" t="n">
-        <v>137045.0</v>
+        <v>664094.0</v>
       </c>
       <c r="G5" t="n">
-        <v>264430.0</v>
+        <v>207680.0</v>
       </c>
       <c r="H5" t="n">
-        <v>307898.0</v>
+        <v>213114.0</v>
       </c>
       <c r="I5" t="n">
-        <v>357403.0</v>
+        <v>307295.0</v>
       </c>
     </row>
     <row r="6">
@@ -2264,28 +2264,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>1409087.0</v>
+        <v>1840748.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1546736.0</v>
+        <v>1500852.0</v>
       </c>
       <c r="D6" t="n">
-        <v>2373834.0</v>
+        <v>3885554.0</v>
       </c>
       <c r="E6" t="n">
-        <v>2468015.0</v>
+        <v>2699240.0</v>
       </c>
       <c r="F6" t="n">
-        <v>2940125.0</v>
+        <v>4249598.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1614352.0</v>
+        <v>1705515.0</v>
       </c>
       <c r="H6" t="n">
-        <v>1574506.0</v>
+        <v>1633671.0</v>
       </c>
       <c r="I6" t="n">
-        <v>2003149.0</v>
+        <v>1994093.0</v>
       </c>
     </row>
   </sheetData>
@@ -2339,28 +2339,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>126782.0</v>
+        <v>516182.0</v>
       </c>
       <c r="C2" t="n">
-        <v>1208047.0</v>
+        <v>1485760.0</v>
       </c>
       <c r="D2" t="n">
-        <v>7303826.0</v>
+        <v>3587315.0</v>
       </c>
       <c r="E2" t="n">
-        <v>6081290.0</v>
+        <v>1.5858565E7</v>
       </c>
       <c r="F2" t="n">
-        <v>6873977.0</v>
+        <v>1.1130215E7</v>
       </c>
       <c r="G2" t="n">
-        <v>9742862.0</v>
+        <v>1.6051153E7</v>
       </c>
       <c r="H2" t="n">
-        <v>1.2829088E7</v>
+        <v>2.493673E7</v>
       </c>
       <c r="I2" t="n">
-        <v>2.0793991E7</v>
+        <v>3.0281479E7</v>
       </c>
     </row>
     <row r="3">
@@ -2368,28 +2368,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>260204.0</v>
+        <v>236056.0</v>
       </c>
       <c r="C3" t="n">
-        <v>2054465.0</v>
+        <v>2161928.0</v>
       </c>
       <c r="D3" t="n">
-        <v>6478539.0</v>
+        <v>5903192.0</v>
       </c>
       <c r="E3" t="n">
-        <v>1.6792522E7</v>
+        <v>8618129.0</v>
       </c>
       <c r="F3" t="n">
-        <v>1.7396848E7</v>
+        <v>2.0515072E7</v>
       </c>
       <c r="G3" t="n">
-        <v>2.5691986E7</v>
+        <v>2.4881791E7</v>
       </c>
       <c r="H3" t="n">
-        <v>3.8642423E7</v>
+        <v>5.4312022E7</v>
       </c>
       <c r="I3" t="n">
-        <v>4.3470386E7</v>
+        <v>4.3035707E7</v>
       </c>
     </row>
     <row r="4">
@@ -2397,28 +2397,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>182928.0</v>
+        <v>257789.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1560018.0</v>
+        <v>2037561.0</v>
       </c>
       <c r="D4" t="n">
-        <v>5524055.0</v>
+        <v>6484577.0</v>
       </c>
       <c r="E4" t="n">
-        <v>8834865.0</v>
+        <v>9782105.0</v>
       </c>
       <c r="F4" t="n">
-        <v>1.3412284E7</v>
+        <v>2.0806066E7</v>
       </c>
       <c r="G4" t="n">
-        <v>1.7407111E7</v>
+        <v>2.762631E7</v>
       </c>
       <c r="H4" t="n">
-        <v>2.660904E7</v>
+        <v>4.5178919E7</v>
       </c>
       <c r="I4" t="n">
-        <v>3.3303711E7</v>
+        <v>4.2182647E7</v>
       </c>
     </row>
     <row r="5">
@@ -2426,28 +2426,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>25960.0</v>
+        <v>22941.0</v>
       </c>
       <c r="C5" t="n">
-        <v>58561.0</v>
+        <v>45883.0</v>
       </c>
       <c r="D5" t="n">
-        <v>81503.0</v>
+        <v>138253.0</v>
       </c>
       <c r="E5" t="n">
-        <v>36827.0</v>
+        <v>33205.0</v>
       </c>
       <c r="F5" t="n">
-        <v>22338.0</v>
+        <v>29582.0</v>
       </c>
       <c r="G5" t="n">
-        <v>34412.0</v>
+        <v>35016.0</v>
       </c>
       <c r="H5" t="n">
-        <v>43468.0</v>
+        <v>42864.0</v>
       </c>
       <c r="I5" t="n">
-        <v>45883.0</v>
+        <v>52523.0</v>
       </c>
     </row>
     <row r="6">
@@ -2455,28 +2455,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>123160.0</v>
+        <v>111689.0</v>
       </c>
       <c r="C6" t="n">
-        <v>350762.0</v>
+        <v>420794.0</v>
       </c>
       <c r="D6" t="n">
-        <v>575951.0</v>
+        <v>560254.0</v>
       </c>
       <c r="E6" t="n">
-        <v>588629.0</v>
+        <v>534897.0</v>
       </c>
       <c r="F6" t="n">
-        <v>709977.0</v>
+        <v>907394.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1197180.0</v>
+        <v>1345092.0</v>
       </c>
       <c r="H6" t="n">
-        <v>1654198.0</v>
+        <v>1075833.0</v>
       </c>
       <c r="I6" t="n">
-        <v>1889649.0</v>
+        <v>2110008.0</v>
       </c>
     </row>
   </sheetData>
@@ -2501,28 +2501,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>500.0</v>
+        <v>501.0</v>
       </c>
       <c r="C1" t="n">
-        <v>1500.0</v>
+        <v>1501.0</v>
       </c>
       <c r="D1" t="n">
-        <v>2500.0</v>
+        <v>2501.0</v>
       </c>
       <c r="E1" t="n">
-        <v>3500.0</v>
+        <v>3501.0</v>
       </c>
       <c r="F1" t="n">
-        <v>4500.0</v>
+        <v>4501.0</v>
       </c>
       <c r="G1" t="n">
-        <v>5500.0</v>
+        <v>5501.0</v>
       </c>
       <c r="H1" t="n">
-        <v>6500.0</v>
+        <v>6501.0</v>
       </c>
       <c r="I1" t="n">
-        <v>7500.0</v>
+        <v>7501.0</v>
       </c>
     </row>
     <row r="2">
@@ -2530,28 +2530,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>388193.0</v>
+        <v>173268.0</v>
       </c>
       <c r="C2" t="n">
-        <v>2926240.0</v>
+        <v>1267816.0</v>
       </c>
       <c r="D2" t="n">
-        <v>1.8002985E7</v>
+        <v>3139353.0</v>
       </c>
       <c r="E2" t="n">
-        <v>2.2884679E7</v>
+        <v>7723414.0</v>
       </c>
       <c r="F2" t="n">
-        <v>3.1544465E7</v>
+        <v>1.0256027E7</v>
       </c>
       <c r="G2" t="n">
-        <v>5.0991553E7</v>
+        <v>1.593403E7</v>
       </c>
       <c r="H2" t="n">
-        <v>8.7344058E7</v>
+        <v>6.5366773E7</v>
       </c>
       <c r="I2" t="n">
-        <v>2.06484334E8</v>
+        <v>5.5798989E7</v>
       </c>
     </row>
     <row r="3">
@@ -2559,28 +2559,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>574743.0</v>
+        <v>255374.0</v>
       </c>
       <c r="C3" t="n">
-        <v>4326875.0</v>
+        <v>1815392.0</v>
       </c>
       <c r="D3" t="n">
-        <v>1.4014798E7</v>
+        <v>5282566.0</v>
       </c>
       <c r="E3" t="n">
-        <v>2.0932243E7</v>
+        <v>1.1332462E7</v>
       </c>
       <c r="F3" t="n">
-        <v>5.0450014E7</v>
+        <v>1.3574686E7</v>
       </c>
       <c r="G3" t="n">
-        <v>6.4194346E7</v>
+        <v>2.3678574E7</v>
       </c>
       <c r="H3" t="n">
-        <v>1.06966829E8</v>
+        <v>7.8494704E7</v>
       </c>
       <c r="I3" t="n">
-        <v>1.78788596E8</v>
+        <v>5.697021E7</v>
       </c>
     </row>
     <row r="4">
@@ -2588,28 +2588,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>225188.0</v>
+        <v>255374.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1595033.0</v>
+        <v>2270598.0</v>
       </c>
       <c r="D4" t="n">
-        <v>4512217.0</v>
+        <v>5560882.0</v>
       </c>
       <c r="E4" t="n">
-        <v>6502084.0</v>
+        <v>1.1256394E7</v>
       </c>
       <c r="F4" t="n">
-        <v>1.0304324E7</v>
+        <v>1.3747954E7</v>
       </c>
       <c r="G4" t="n">
-        <v>1.562915E7</v>
+        <v>4.0119126E7</v>
       </c>
       <c r="H4" t="n">
-        <v>3.4183333E7</v>
+        <v>4.9900628E7</v>
       </c>
       <c r="I4" t="n">
-        <v>4.9322866E7</v>
+        <v>9.9078599E7</v>
       </c>
     </row>
     <row r="5">
@@ -2617,28 +2617,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>36224.0</v>
+        <v>10264.0</v>
       </c>
       <c r="C5" t="n">
-        <v>64599.0</v>
+        <v>15093.0</v>
       </c>
       <c r="D5" t="n">
-        <v>99011.0</v>
+        <v>20527.0</v>
       </c>
       <c r="E5" t="n">
-        <v>111085.0</v>
+        <v>22941.0</v>
       </c>
       <c r="F5" t="n">
-        <v>102029.0</v>
+        <v>32601.0</v>
       </c>
       <c r="G5" t="n">
-        <v>123763.0</v>
+        <v>38638.0</v>
       </c>
       <c r="H5" t="n">
-        <v>247526.0</v>
+        <v>1887234.0</v>
       </c>
       <c r="I5" t="n">
-        <v>211303.0</v>
+        <v>65806.0</v>
       </c>
     </row>
     <row r="6">
@@ -2646,28 +2646,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>127989.0</v>
+        <v>103236.0</v>
       </c>
       <c r="C6" t="n">
-        <v>386382.0</v>
+        <v>302465.0</v>
       </c>
       <c r="D6" t="n">
-        <v>1297399.0</v>
+        <v>674358.0</v>
       </c>
       <c r="E6" t="n">
-        <v>962937.0</v>
+        <v>868756.0</v>
       </c>
       <c r="F6" t="n">
-        <v>839173.0</v>
+        <v>1203218.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1590203.0</v>
+        <v>1345695.0</v>
       </c>
       <c r="H6" t="n">
-        <v>1801506.0</v>
+        <v>1450743.0</v>
       </c>
       <c r="I6" t="n">
-        <v>2166758.0</v>
+        <v>2476467.0</v>
       </c>
     </row>
   </sheetData>
@@ -2721,28 +2721,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>307898.0</v>
+        <v>396645.0</v>
       </c>
       <c r="C2" t="n">
-        <v>3337374.0</v>
+        <v>5429875.0</v>
       </c>
       <c r="D2" t="n">
-        <v>7883400.0</v>
+        <v>9495337.0</v>
       </c>
       <c r="E2" t="n">
-        <v>2.3613976E7</v>
+        <v>2.1540795E7</v>
       </c>
       <c r="F2" t="n">
-        <v>2.8520422E7</v>
+        <v>6.936643E7</v>
       </c>
       <c r="G2" t="n">
-        <v>2.3894102E7</v>
+        <v>5.5711449E7</v>
       </c>
       <c r="H2" t="n">
-        <v>3.4925307E7</v>
+        <v>7.9525257E7</v>
       </c>
       <c r="I2" t="n">
-        <v>3.7742273E7</v>
+        <v>9.1576753E7</v>
       </c>
     </row>
     <row r="3">
@@ -2750,28 +2750,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>469092.0</v>
+        <v>239074.0</v>
       </c>
       <c r="C3" t="n">
-        <v>9057034.0</v>
+        <v>1692836.0</v>
       </c>
       <c r="D3" t="n">
-        <v>1.2393806E7</v>
+        <v>5853687.0</v>
       </c>
       <c r="E3" t="n">
-        <v>2.5669044E7</v>
+        <v>1.374735E7</v>
       </c>
       <c r="F3" t="n">
-        <v>4.721648E7</v>
+        <v>4.7386126E7</v>
       </c>
       <c r="G3" t="n">
-        <v>4.9689325E7</v>
+        <v>4.3333342E7</v>
       </c>
       <c r="H3" t="n">
-        <v>8.5781626E7</v>
+        <v>4.2420514E7</v>
       </c>
       <c r="I3" t="n">
-        <v>8.046646E7</v>
+        <v>3.0294761E7</v>
       </c>
     </row>
     <row r="4">
@@ -2779,28 +2779,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>199832.0</v>
+        <v>717825.0</v>
       </c>
       <c r="C4" t="n">
-        <v>2714333.0</v>
+        <v>4488672.0</v>
       </c>
       <c r="D4" t="n">
-        <v>4349212.0</v>
+        <v>1.7089554E7</v>
       </c>
       <c r="E4" t="n">
-        <v>8402600.0</v>
+        <v>2.3644765E7</v>
       </c>
       <c r="F4" t="n">
-        <v>1.6305923E7</v>
+        <v>6.7821506E7</v>
       </c>
       <c r="G4" t="n">
-        <v>3.7183227E7</v>
+        <v>8.182423E7</v>
       </c>
       <c r="H4" t="n">
-        <v>2.7976469E7</v>
+        <v>9.5042115E7</v>
       </c>
       <c r="I4" t="n">
-        <v>2.8607359E7</v>
+        <v>1.06106526E8</v>
       </c>
     </row>
     <row r="5">
@@ -2808,28 +2808,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>13282.0</v>
+        <v>38034.0</v>
       </c>
       <c r="C5" t="n">
-        <v>21130.0</v>
+        <v>63391.0</v>
       </c>
       <c r="D5" t="n">
-        <v>26563.0</v>
+        <v>82710.0</v>
       </c>
       <c r="E5" t="n">
-        <v>38035.0</v>
+        <v>101426.0</v>
       </c>
       <c r="F5" t="n">
-        <v>45279.0</v>
+        <v>136441.0</v>
       </c>
       <c r="G5" t="n">
-        <v>144894.0</v>
+        <v>159986.0</v>
       </c>
       <c r="H5" t="n">
-        <v>37431.0</v>
+        <v>193191.0</v>
       </c>
       <c r="I5" t="n">
-        <v>71239.0</v>
+        <v>137649.0</v>
       </c>
     </row>
     <row r="6">
@@ -2837,28 +2837,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>115311.0</v>
+        <v>124971.0</v>
       </c>
       <c r="C6" t="n">
-        <v>340499.0</v>
+        <v>382759.0</v>
       </c>
       <c r="D6" t="n">
-        <v>901356.0</v>
+        <v>734729.0</v>
       </c>
       <c r="E6" t="n">
-        <v>868152.0</v>
+        <v>1051080.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1042024.0</v>
+        <v>1250912.0</v>
       </c>
       <c r="G6" t="n">
-        <v>2379268.0</v>
+        <v>1491193.0</v>
       </c>
       <c r="H6" t="n">
-        <v>1226762.0</v>
+        <v>1723625.0</v>
       </c>
       <c r="I6" t="n">
-        <v>1846785.0</v>
+        <v>1331207.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimaze and bugfix CreateFillExcel
</commit_message>
<xml_diff>
--- a/arrays.xlsx
+++ b/arrays.xlsx
@@ -6,9 +6,9 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Random Array" r:id="rId3" sheetId="1"/>
-    <sheet name="Sorted Array(Min to Max)" r:id="rId4" sheetId="2"/>
-    <sheet name="Sorted Array(Min to Max) + 1" r:id="rId5" sheetId="3"/>
+    <sheet name="Sorted Array(Min to Max) + 1" r:id="rId3" sheetId="1"/>
+    <sheet name="Random Array" r:id="rId4" sheetId="2"/>
+    <sheet name="Sorted Array(Min to Max)" r:id="rId5" sheetId="3"/>
     <sheet name="Sorted Array(Max to Min)" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
@@ -20,13 +20,13 @@
     <t>Length of array</t>
   </si>
   <si>
-    <t>Selection Sort</t>
-  </si>
-  <si>
     <t>Bubble Sort (Down)</t>
   </si>
   <si>
     <t>Bubble Sort (Up)</t>
+  </si>
+  <si>
+    <t>Selection Sort</t>
   </si>
   <si>
     <t>Native Sort</t>
@@ -84,7 +84,7 @@
           <a:bodyPr/>
           <a:p>
             <a:r>
-              <a:t>Random Array</a:t>
+              <a:t>Sorted Array(Min to Max) + 1</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -98,80 +98,6 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Selection Sort</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Random Array'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1500.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10500.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12000.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Random Array'!$B$2:$I$2</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>9501363.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7253746E7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.1406742E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.8961926E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.7013754E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.19053196E8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.08108698E8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.54332243E8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
             <c:v>Bubble Sort (Down)</c:v>
           </c:tx>
           <c:marker>
@@ -179,72 +105,72 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Random Array'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1500.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10500.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12000.0</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1501.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3001.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4501.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6001.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7501.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9001.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10501.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12001.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Random Array'!$B$3:$I$3</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1.4970472E7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.9637912E7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.4252757E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.82059341E8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.54102586E8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.44367704E8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.03635246E8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.93976675E8</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$2:$I$2</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9409597.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7225938.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1971825E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.05083694E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8547665E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3975721E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.1245199E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.63843868E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Bubble Sort (Up)</c:v>
           </c:tx>
@@ -253,64 +179,138 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Random Array'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1500.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10500.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12000.0</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1501.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3001.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4501.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6001.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7501.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9001.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10501.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12001.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Random Array'!$B$4:$I$4</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1.3080825E7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.7568924E7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.8575327E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.15178514E8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.92762712E8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.37029475E8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.67542022E8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.58505283E8</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9725946.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9893214E7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1535299E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0161109E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.9263182E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.43529861E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.93459407E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.63966907E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Selection Sort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1501.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3001.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4501.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6001.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7501.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9001.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10501.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12001.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$4:$I$4</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.5182378E7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9767000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2163773E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1682039E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2235688E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.301939E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0478365E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.8490456E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -327,64 +327,64 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Random Array'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1500.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10500.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12000.0</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1501.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3001.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4501.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6001.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7501.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9001.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10501.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12001.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Random Array'!$B$5:$I$5</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1750188.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>523426.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>737747.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1179671.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>942409.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>507126.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>347743.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>518597.0</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$5:$I$5</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>179908.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>295823.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>503504.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>202246.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>260808.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>604929.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>371893.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>522219.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -401,64 +401,64 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Random Array'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1500.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10500.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12000.0</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1501.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3001.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4501.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6001.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7501.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9001.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10501.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12001.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Random Array'!$B$6:$I$6</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2765042.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3468981.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2833867.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2029710.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1829275.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2605057.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2169170.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2253691.0</c:v>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$6:$I$6</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2267577.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3362123.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6054718.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1988053.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1901118.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2260332.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2726405.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2890013.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -556,7 +556,7 @@
           <a:bodyPr/>
           <a:p>
             <a:r>
-              <a:t>Sorted Array(Min to Max)</a:t>
+              <a:t>Random Array</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -570,80 +570,6 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Selection Sort</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1500.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10500.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12000.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$2:$I$2</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>6582975.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6070416.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.3487129E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.2113096E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.1778067E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.1436434E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.0521229E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.8539285E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
             <c:v>Bubble Sort (Down)</c:v>
           </c:tx>
           <c:marker>
@@ -651,7 +577,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$1:$I$1</c:f>
+              <c:f>'Random Array'!$B$1:$I$1</c:f>
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -683,40 +609,40 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$3:$I$3</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>6368653.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7233182.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.753508E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.423095E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.7005688E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.6906147E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.0596126E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.601037E7</c:v>
+              <c:f>'Random Array'!$B$2:$I$2</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3751523.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7425806E7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2139165E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.09536741E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.29135339E8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.64884683E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.43497622E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.12930981E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Bubble Sort (Up)</c:v>
           </c:tx>
@@ -725,7 +651,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$1:$I$1</c:f>
+              <c:f>'Random Array'!$B$1:$I$1</c:f>
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -757,32 +683,106 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$4:$I$4</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>3188251.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4736796.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.1330637E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.8401419E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.6559502E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.936503E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.3484859E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6.8589961E7</c:v>
+              <c:f>'Random Array'!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.8536048E7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3454528E7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9362012E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4584912E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.0558128E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.20190607E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.05306346E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.34266727E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Selection Sort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Random Array'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Random Array'!$B$4:$I$4</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1645140.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4436746.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4955379E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.774521E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8005414E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.9964526E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.14546419E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1030202E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -799,7 +799,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$1:$I$1</c:f>
+              <c:f>'Random Array'!$B$1:$I$1</c:f>
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -831,32 +831,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$5:$I$5</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>207076.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>214925.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>48901.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>27771.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30186.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>35619.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>40449.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>539123.0</c:v>
+              <c:f>'Random Array'!$B$5:$I$5</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>108669.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>230622.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>142478.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>158175.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>144289.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>166627.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>485392.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>271071.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -873,7 +873,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$1:$I$1</c:f>
+              <c:f>'Random Array'!$B$1:$I$1</c:f>
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -905,32 +905,32 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$6:$I$6</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>332650.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>505918.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>670130.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>932145.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1289548.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1357768.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1705512.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2704671.0</c:v>
+              <c:f>'Random Array'!$B$6:$I$6</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>403889.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>877207.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1156729.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1805126.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1362599.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1598050.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4213369.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3333144.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1028,7 +1028,7 @@
           <a:bodyPr/>
           <a:p>
             <a:r>
-              <a:t>Sorted Array(Min to Max) + 1</a:t>
+              <a:t>Sorted Array(Min to Max)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1042,80 +1042,6 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Selection Sort</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1501.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3001.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4501.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6001.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7501.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9001.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10501.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12001.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$2:$I$2</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1105414.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6145277.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.3726203E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.9096302E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.2079928E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.2005103E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.7713926E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.6187791E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
             <c:v>Bubble Sort (Down)</c:v>
           </c:tx>
           <c:marker>
@@ -1123,72 +1049,72 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1501.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3001.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4501.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6001.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7501.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9001.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10501.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12001.0</c:v>
+              <c:f>'Sorted Array(Min to Max)'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$3:$I$3</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1493606.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7445692.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.3230547E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.3633266E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.524403E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.0112473E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.021216E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.2126631E7</c:v>
+              <c:f>'Sorted Array(Min to Max)'!$B$2:$I$2</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1329997.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6130788.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.278138E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6908453E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6467773E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1166571E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.948528E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0966883E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Bubble Sort (Up)</c:v>
           </c:tx>
@@ -1197,64 +1123,138 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1501.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3001.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4501.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6001.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7501.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9001.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10501.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12001.0</c:v>
+              <c:f>'Sorted Array(Min to Max)'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$4:$I$4</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1075228.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4689102.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0140099E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.7137227E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.6977277E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.0135378E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.3288046E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6.8762021E7</c:v>
+              <c:f>'Sorted Array(Min to Max)'!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>668319.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4643219.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6717001.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1670533E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8010208E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6164669E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.7512211E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5405864E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Selection Sort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sorted Array(Min to Max)'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sorted Array(Min to Max)'!$B$4:$I$4</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1236421.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4066665.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9543623.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7911801E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1947109E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0680539E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3573003E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.260531E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1271,64 +1271,64 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1501.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3001.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4501.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6001.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7501.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9001.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10501.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12001.0</c:v>
+              <c:f>'Sorted Array(Min to Max)'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$5:$I$5</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>81502.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>94784.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>38638.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25356.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30187.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
+              <c:f>'Sorted Array(Min to Max)'!$B$5:$I$5</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>13886.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16904.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20526.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>38034.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>42865.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44675.0</c:v>
+                <c:pt idx="4">
+                  <c:v>32601.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1312490.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42261.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47694.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1345,64 +1345,64 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1501.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3001.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4501.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6001.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7501.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9001.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10501.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12001.0</c:v>
+              <c:f>'Sorted Array(Min to Max)'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$6:$I$6</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>214321.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>678583.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>979839.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>858491.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1078849.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1437460.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1647555.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2037559.0</c:v>
+              <c:f>'Sorted Array(Min to Max)'!$B$6:$I$6</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>338688.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>459432.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>657453.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>888677.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1069794.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1351732.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1819012.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2084649.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1514,80 +1514,6 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Selection Sort</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$1:$I$1</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1500.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7500.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10500.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12000.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$2:$I$2</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1476098.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5008470.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0955727E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.8833684E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.3300652E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.2546036E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.3356303E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0931228E7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
             <c:v>Bubble Sort (Down)</c:v>
           </c:tx>
           <c:marker>
@@ -1627,40 +1553,40 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$3:$I$3</c:f>
-              <c:numCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>3072336.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.2388961E7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.8210075E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.9555239E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.4656754E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.11812165E8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.50967705E8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.92766938E8</c:v>
+              <c:f>'Sorted Array(Max to Min)'!$B$2:$I$2</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2978156.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4480855E7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6473774E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7474212E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.692433E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.10637928E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.43739956E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.19889712E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Bubble Sort (Up)</c:v>
           </c:tx>
@@ -1701,32 +1627,106 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:f>'Sorted Array(Max to Min)'!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1636688.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5466695.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1389199E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9828012E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3898939E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7879912E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.1801721E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.2561878E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Selection Sort</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sorted Array(Max to Min)'!$B$1:$I$1</c:f>
+              <c:numCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7500.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10500.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
               <c:f>'Sorted Array(Max to Min)'!$B$4:$I$4</c:f>
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1061946.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4453650.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0676807E7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.7471085E7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.3217338E7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.6543275E7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.3573606E7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.2566069E7</c:v>
+                  <c:v>1117488.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4348603.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0183568E7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1908435E7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6979692E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7706005E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4257623E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.4537218E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1779,28 +1779,28 @@
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>12678.0</c:v>
+                  <c:v>13885.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>19319.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27771.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>31393.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40450.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42261.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>49505.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>55542.0</c:v>
+                  <c:v>27167.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53731.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38034.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47694.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50712.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57957.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1853,28 +1853,28 @@
               <c:numCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>202246.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>568102.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>664697.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1189934.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1241854.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1698871.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1566053.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2040578.0</c:v>
+                  <c:v>216736.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>412945.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>633907.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1595635.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1080057.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1425990.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1725434.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1935530.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2119,28 +2119,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>1500.0</v>
+        <v>1501.0</v>
       </c>
       <c r="C1" t="n">
-        <v>3000.0</v>
+        <v>3001.0</v>
       </c>
       <c r="D1" t="n">
-        <v>4500.0</v>
+        <v>4501.0</v>
       </c>
       <c r="E1" t="n">
-        <v>6000.0</v>
+        <v>6001.0</v>
       </c>
       <c r="F1" t="n">
-        <v>7500.0</v>
+        <v>7501.0</v>
       </c>
       <c r="G1" t="n">
-        <v>9000.0</v>
+        <v>9001.0</v>
       </c>
       <c r="H1" t="n">
-        <v>10500.0</v>
+        <v>10501.0</v>
       </c>
       <c r="I1" t="n">
-        <v>12000.0</v>
+        <v>12001.0</v>
       </c>
     </row>
     <row r="2">
@@ -2148,28 +2148,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>9501363.0</v>
+        <v>9409597.0</v>
       </c>
       <c r="C2" t="n">
-        <v>1.7253746E7</v>
+        <v>7225938.0</v>
       </c>
       <c r="D2" t="n">
-        <v>2.1406742E7</v>
+        <v>2.1971825E7</v>
       </c>
       <c r="E2" t="n">
-        <v>8.8961926E7</v>
+        <v>1.05083694E8</v>
       </c>
       <c r="F2" t="n">
-        <v>9.7013754E7</v>
+        <v>5.8547665E7</v>
       </c>
       <c r="G2" t="n">
-        <v>1.19053196E8</v>
+        <v>6.3975721E7</v>
       </c>
       <c r="H2" t="n">
-        <v>2.08108698E8</v>
+        <v>9.1245199E7</v>
       </c>
       <c r="I2" t="n">
-        <v>1.54332243E8</v>
+        <v>1.63843868E8</v>
       </c>
     </row>
     <row r="3">
@@ -2177,28 +2177,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>1.4970472E7</v>
+        <v>9725946.0</v>
       </c>
       <c r="C3" t="n">
-        <v>3.9637912E7</v>
+        <v>1.9893214E7</v>
       </c>
       <c r="D3" t="n">
-        <v>4.4252757E7</v>
+        <v>1.1535299E7</v>
       </c>
       <c r="E3" t="n">
-        <v>1.82059341E8</v>
+        <v>1.0161109E8</v>
       </c>
       <c r="F3" t="n">
-        <v>2.54102586E8</v>
+        <v>8.9263182E7</v>
       </c>
       <c r="G3" t="n">
-        <v>4.44367704E8</v>
+        <v>1.43529861E8</v>
       </c>
       <c r="H3" t="n">
-        <v>4.03635246E8</v>
+        <v>1.93459407E8</v>
       </c>
       <c r="I3" t="n">
-        <v>4.93976675E8</v>
+        <v>4.63966907E8</v>
       </c>
     </row>
     <row r="4">
@@ -2206,28 +2206,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>1.3080825E7</v>
+        <v>1.5182378E7</v>
       </c>
       <c r="C4" t="n">
-        <v>2.7568924E7</v>
+        <v>9767000.0</v>
       </c>
       <c r="D4" t="n">
-        <v>2.8575327E7</v>
+        <v>1.2163773E7</v>
       </c>
       <c r="E4" t="n">
-        <v>1.15178514E8</v>
+        <v>2.1682039E7</v>
       </c>
       <c r="F4" t="n">
-        <v>1.92762712E8</v>
+        <v>3.2235688E7</v>
       </c>
       <c r="G4" t="n">
-        <v>4.37029475E8</v>
+        <v>5.301939E7</v>
       </c>
       <c r="H4" t="n">
-        <v>2.67542022E8</v>
+        <v>6.0478365E7</v>
       </c>
       <c r="I4" t="n">
-        <v>3.58505283E8</v>
+        <v>9.8490456E7</v>
       </c>
     </row>
     <row r="5">
@@ -2235,28 +2235,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>1750188.0</v>
+        <v>179908.0</v>
       </c>
       <c r="C5" t="n">
-        <v>523426.0</v>
+        <v>295823.0</v>
       </c>
       <c r="D5" t="n">
-        <v>737747.0</v>
+        <v>503504.0</v>
       </c>
       <c r="E5" t="n">
-        <v>1179671.0</v>
+        <v>202246.0</v>
       </c>
       <c r="F5" t="n">
-        <v>942409.0</v>
+        <v>260808.0</v>
       </c>
       <c r="G5" t="n">
-        <v>507126.0</v>
+        <v>604929.0</v>
       </c>
       <c r="H5" t="n">
-        <v>347743.0</v>
+        <v>371893.0</v>
       </c>
       <c r="I5" t="n">
-        <v>518597.0</v>
+        <v>522219.0</v>
       </c>
     </row>
     <row r="6">
@@ -2264,28 +2264,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>2765042.0</v>
+        <v>2267577.0</v>
       </c>
       <c r="C6" t="n">
-        <v>3468981.0</v>
+        <v>3362123.0</v>
       </c>
       <c r="D6" t="n">
-        <v>2833867.0</v>
+        <v>6054718.0</v>
       </c>
       <c r="E6" t="n">
-        <v>2029710.0</v>
+        <v>1988053.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1829275.0</v>
+        <v>1901118.0</v>
       </c>
       <c r="G6" t="n">
-        <v>2605057.0</v>
+        <v>2260332.0</v>
       </c>
       <c r="H6" t="n">
-        <v>2169170.0</v>
+        <v>2726405.0</v>
       </c>
       <c r="I6" t="n">
-        <v>2253691.0</v>
+        <v>2890013.0</v>
       </c>
     </row>
   </sheetData>
@@ -2339,28 +2339,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>6582975.0</v>
+        <v>3751523.0</v>
       </c>
       <c r="C2" t="n">
-        <v>6070416.0</v>
+        <v>1.7425806E7</v>
       </c>
       <c r="D2" t="n">
-        <v>1.3487129E7</v>
+        <v>5.2139165E7</v>
       </c>
       <c r="E2" t="n">
-        <v>2.2113096E7</v>
+        <v>1.09536741E8</v>
       </c>
       <c r="F2" t="n">
-        <v>3.1778067E7</v>
+        <v>1.29135339E8</v>
       </c>
       <c r="G2" t="n">
-        <v>5.1436434E7</v>
+        <v>1.64884683E8</v>
       </c>
       <c r="H2" t="n">
-        <v>6.0521229E7</v>
+        <v>2.43497622E8</v>
       </c>
       <c r="I2" t="n">
-        <v>7.8539285E7</v>
+        <v>3.12930981E8</v>
       </c>
     </row>
     <row r="3">
@@ -2368,28 +2368,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>6368653.0</v>
+        <v>1.8536048E7</v>
       </c>
       <c r="C3" t="n">
-        <v>7233182.0</v>
+        <v>1.3454528E7</v>
       </c>
       <c r="D3" t="n">
-        <v>1.753508E7</v>
+        <v>3.9362012E7</v>
       </c>
       <c r="E3" t="n">
-        <v>2.423095E7</v>
+        <v>7.4584912E7</v>
       </c>
       <c r="F3" t="n">
-        <v>3.7005688E7</v>
+        <v>8.0558128E7</v>
       </c>
       <c r="G3" t="n">
-        <v>5.6906147E7</v>
+        <v>1.20190607E8</v>
       </c>
       <c r="H3" t="n">
-        <v>7.0596126E7</v>
+        <v>4.05306346E8</v>
       </c>
       <c r="I3" t="n">
-        <v>9.601037E7</v>
+        <v>2.34266727E8</v>
       </c>
     </row>
     <row r="4">
@@ -2397,28 +2397,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3188251.0</v>
+        <v>1645140.0</v>
       </c>
       <c r="C4" t="n">
-        <v>4736796.0</v>
+        <v>4436746.0</v>
       </c>
       <c r="D4" t="n">
-        <v>1.1330637E7</v>
+        <v>1.4955379E7</v>
       </c>
       <c r="E4" t="n">
-        <v>1.8401419E7</v>
+        <v>2.774521E7</v>
       </c>
       <c r="F4" t="n">
-        <v>2.6559502E7</v>
+        <v>2.8005414E7</v>
       </c>
       <c r="G4" t="n">
-        <v>3.936503E7</v>
+        <v>3.9964526E7</v>
       </c>
       <c r="H4" t="n">
-        <v>5.3484859E7</v>
+        <v>1.14546419E8</v>
       </c>
       <c r="I4" t="n">
-        <v>6.8589961E7</v>
+        <v>7.1030202E7</v>
       </c>
     </row>
     <row r="5">
@@ -2426,28 +2426,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>207076.0</v>
+        <v>108669.0</v>
       </c>
       <c r="C5" t="n">
-        <v>214925.0</v>
+        <v>230622.0</v>
       </c>
       <c r="D5" t="n">
-        <v>48901.0</v>
+        <v>142478.0</v>
       </c>
       <c r="E5" t="n">
-        <v>27771.0</v>
+        <v>158175.0</v>
       </c>
       <c r="F5" t="n">
-        <v>30186.0</v>
+        <v>144289.0</v>
       </c>
       <c r="G5" t="n">
-        <v>35619.0</v>
+        <v>166627.0</v>
       </c>
       <c r="H5" t="n">
-        <v>40449.0</v>
+        <v>485392.0</v>
       </c>
       <c r="I5" t="n">
-        <v>539123.0</v>
+        <v>271071.0</v>
       </c>
     </row>
     <row r="6">
@@ -2455,28 +2455,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>332650.0</v>
+        <v>403889.0</v>
       </c>
       <c r="C6" t="n">
-        <v>505918.0</v>
+        <v>877207.0</v>
       </c>
       <c r="D6" t="n">
-        <v>670130.0</v>
+        <v>1156729.0</v>
       </c>
       <c r="E6" t="n">
-        <v>932145.0</v>
+        <v>1805126.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1289548.0</v>
+        <v>1362599.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1357768.0</v>
+        <v>1598050.0</v>
       </c>
       <c r="H6" t="n">
-        <v>1705512.0</v>
+        <v>4213369.0</v>
       </c>
       <c r="I6" t="n">
-        <v>2704671.0</v>
+        <v>3333144.0</v>
       </c>
     </row>
   </sheetData>
@@ -2501,28 +2501,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>1501.0</v>
+        <v>1500.0</v>
       </c>
       <c r="C1" t="n">
-        <v>3001.0</v>
+        <v>3000.0</v>
       </c>
       <c r="D1" t="n">
-        <v>4501.0</v>
+        <v>4500.0</v>
       </c>
       <c r="E1" t="n">
-        <v>6001.0</v>
+        <v>6000.0</v>
       </c>
       <c r="F1" t="n">
-        <v>7501.0</v>
+        <v>7500.0</v>
       </c>
       <c r="G1" t="n">
-        <v>9001.0</v>
+        <v>9000.0</v>
       </c>
       <c r="H1" t="n">
-        <v>10501.0</v>
+        <v>10500.0</v>
       </c>
       <c r="I1" t="n">
-        <v>12001.0</v>
+        <v>12000.0</v>
       </c>
     </row>
     <row r="2">
@@ -2530,28 +2530,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1105414.0</v>
+        <v>1329997.0</v>
       </c>
       <c r="C2" t="n">
-        <v>6145277.0</v>
+        <v>6130788.0</v>
       </c>
       <c r="D2" t="n">
-        <v>1.3726203E7</v>
+        <v>1.278138E7</v>
       </c>
       <c r="E2" t="n">
-        <v>1.9096302E7</v>
+        <v>2.6908453E7</v>
       </c>
       <c r="F2" t="n">
-        <v>3.2079928E7</v>
+        <v>3.6467773E7</v>
       </c>
       <c r="G2" t="n">
-        <v>4.2005103E7</v>
+        <v>5.1166571E7</v>
       </c>
       <c r="H2" t="n">
-        <v>5.7713926E7</v>
+        <v>6.948528E7</v>
       </c>
       <c r="I2" t="n">
-        <v>7.6187791E7</v>
+        <v>9.0966883E7</v>
       </c>
     </row>
     <row r="3">
@@ -2559,28 +2559,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>1493606.0</v>
+        <v>668319.0</v>
       </c>
       <c r="C3" t="n">
-        <v>7445692.0</v>
+        <v>4643219.0</v>
       </c>
       <c r="D3" t="n">
-        <v>1.3230547E7</v>
+        <v>6717001.0</v>
       </c>
       <c r="E3" t="n">
-        <v>2.3633266E7</v>
+        <v>1.1670533E7</v>
       </c>
       <c r="F3" t="n">
-        <v>3.524403E7</v>
+        <v>1.8010208E7</v>
       </c>
       <c r="G3" t="n">
-        <v>5.0112473E7</v>
+        <v>2.6164669E7</v>
       </c>
       <c r="H3" t="n">
-        <v>7.021216E7</v>
+        <v>3.7512211E7</v>
       </c>
       <c r="I3" t="n">
-        <v>9.2126631E7</v>
+        <v>4.5405864E7</v>
       </c>
     </row>
     <row r="4">
@@ -2588,28 +2588,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>1075228.0</v>
+        <v>1236421.0</v>
       </c>
       <c r="C4" t="n">
-        <v>4689102.0</v>
+        <v>4066665.0</v>
       </c>
       <c r="D4" t="n">
-        <v>1.0140099E7</v>
+        <v>9543623.0</v>
       </c>
       <c r="E4" t="n">
-        <v>1.7137227E7</v>
+        <v>1.7911801E7</v>
       </c>
       <c r="F4" t="n">
-        <v>2.6977277E7</v>
+        <v>3.1947109E7</v>
       </c>
       <c r="G4" t="n">
-        <v>4.0135378E7</v>
+        <v>4.0680539E7</v>
       </c>
       <c r="H4" t="n">
-        <v>5.3288046E7</v>
+        <v>5.3573003E7</v>
       </c>
       <c r="I4" t="n">
-        <v>6.8762021E7</v>
+        <v>7.260531E7</v>
       </c>
     </row>
     <row r="5">
@@ -2617,28 +2617,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>81502.0</v>
+        <v>13886.0</v>
       </c>
       <c r="C5" t="n">
-        <v>94784.0</v>
+        <v>16904.0</v>
       </c>
       <c r="D5" t="n">
-        <v>38638.0</v>
+        <v>20526.0</v>
       </c>
       <c r="E5" t="n">
-        <v>25356.0</v>
+        <v>38034.0</v>
       </c>
       <c r="F5" t="n">
-        <v>30187.0</v>
+        <v>32601.0</v>
       </c>
       <c r="G5" t="n">
-        <v>38034.0</v>
+        <v>1312490.0</v>
       </c>
       <c r="H5" t="n">
-        <v>42865.0</v>
+        <v>42261.0</v>
       </c>
       <c r="I5" t="n">
-        <v>44675.0</v>
+        <v>47694.0</v>
       </c>
     </row>
     <row r="6">
@@ -2646,28 +2646,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>214321.0</v>
+        <v>338688.0</v>
       </c>
       <c r="C6" t="n">
-        <v>678583.0</v>
+        <v>459432.0</v>
       </c>
       <c r="D6" t="n">
-        <v>979839.0</v>
+        <v>657453.0</v>
       </c>
       <c r="E6" t="n">
-        <v>858491.0</v>
+        <v>888677.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1078849.0</v>
+        <v>1069794.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1437460.0</v>
+        <v>1351732.0</v>
       </c>
       <c r="H6" t="n">
-        <v>1647555.0</v>
+        <v>1819012.0</v>
       </c>
       <c r="I6" t="n">
-        <v>2037559.0</v>
+        <v>2084649.0</v>
       </c>
     </row>
   </sheetData>
@@ -2721,28 +2721,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1476098.0</v>
+        <v>2978156.0</v>
       </c>
       <c r="C2" t="n">
-        <v>5008470.0</v>
+        <v>1.4480855E7</v>
       </c>
       <c r="D2" t="n">
-        <v>1.0955727E7</v>
+        <v>2.6473774E7</v>
       </c>
       <c r="E2" t="n">
-        <v>1.8833684E7</v>
+        <v>4.7474212E7</v>
       </c>
       <c r="F2" t="n">
-        <v>3.3300652E7</v>
+        <v>7.692433E7</v>
       </c>
       <c r="G2" t="n">
-        <v>4.2546036E7</v>
+        <v>1.10637928E8</v>
       </c>
       <c r="H2" t="n">
-        <v>6.3356303E7</v>
+        <v>1.43739956E8</v>
       </c>
       <c r="I2" t="n">
-        <v>8.0931228E7</v>
+        <v>2.19889712E8</v>
       </c>
     </row>
     <row r="3">
@@ -2750,28 +2750,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3072336.0</v>
+        <v>1636688.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.2388961E7</v>
+        <v>5466695.0</v>
       </c>
       <c r="D3" t="n">
-        <v>2.8210075E7</v>
+        <v>1.1389199E7</v>
       </c>
       <c r="E3" t="n">
-        <v>4.9555239E7</v>
+        <v>1.9828012E7</v>
       </c>
       <c r="F3" t="n">
-        <v>7.4656754E7</v>
+        <v>3.3898939E7</v>
       </c>
       <c r="G3" t="n">
-        <v>1.11812165E8</v>
+        <v>4.7879912E7</v>
       </c>
       <c r="H3" t="n">
-        <v>1.50967705E8</v>
+        <v>6.1801721E7</v>
       </c>
       <c r="I3" t="n">
-        <v>1.92766938E8</v>
+        <v>8.2561878E7</v>
       </c>
     </row>
     <row r="4">
@@ -2779,28 +2779,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>1061946.0</v>
+        <v>1117488.0</v>
       </c>
       <c r="C4" t="n">
-        <v>4453650.0</v>
+        <v>4348603.0</v>
       </c>
       <c r="D4" t="n">
-        <v>1.0676807E7</v>
+        <v>1.0183568E7</v>
       </c>
       <c r="E4" t="n">
-        <v>1.7471085E7</v>
+        <v>2.1908435E7</v>
       </c>
       <c r="F4" t="n">
-        <v>3.3217338E7</v>
+        <v>2.6979692E7</v>
       </c>
       <c r="G4" t="n">
-        <v>4.6543275E7</v>
+        <v>3.7706005E7</v>
       </c>
       <c r="H4" t="n">
-        <v>5.3573606E7</v>
+        <v>5.4257623E7</v>
       </c>
       <c r="I4" t="n">
-        <v>7.2566069E7</v>
+        <v>7.4537218E7</v>
       </c>
     </row>
     <row r="5">
@@ -2808,28 +2808,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>12678.0</v>
+        <v>13885.0</v>
       </c>
       <c r="C5" t="n">
         <v>19319.0</v>
       </c>
       <c r="D5" t="n">
-        <v>27771.0</v>
+        <v>27167.0</v>
       </c>
       <c r="E5" t="n">
-        <v>31393.0</v>
+        <v>53731.0</v>
       </c>
       <c r="F5" t="n">
-        <v>40450.0</v>
+        <v>38034.0</v>
       </c>
       <c r="G5" t="n">
-        <v>42261.0</v>
+        <v>47694.0</v>
       </c>
       <c r="H5" t="n">
-        <v>49505.0</v>
+        <v>50712.0</v>
       </c>
       <c r="I5" t="n">
-        <v>55542.0</v>
+        <v>57957.0</v>
       </c>
     </row>
     <row r="6">
@@ -2837,28 +2837,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>202246.0</v>
+        <v>216736.0</v>
       </c>
       <c r="C6" t="n">
-        <v>568102.0</v>
+        <v>412945.0</v>
       </c>
       <c r="D6" t="n">
-        <v>664697.0</v>
+        <v>633907.0</v>
       </c>
       <c r="E6" t="n">
-        <v>1189934.0</v>
+        <v>1595635.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1241854.0</v>
+        <v>1080057.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1698871.0</v>
+        <v>1425990.0</v>
       </c>
       <c r="H6" t="n">
-        <v>1566053.0</v>
+        <v>1725434.0</v>
       </c>
       <c r="I6" t="n">
-        <v>2040578.0</v>
+        <v>1935530.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change static methods in CreateFillExcel to non-static Try-catch with resources
</commit_message>
<xml_diff>
--- a/arrays.xlsx
+++ b/arrays.xlsx
@@ -6,10 +6,10 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Random Array" r:id="rId3" sheetId="1"/>
-    <sheet name="Sorted Array(Min to Max) + 1" r:id="rId4" sheetId="2"/>
-    <sheet name="Sorted Array(Min to Max)" r:id="rId5" sheetId="3"/>
-    <sheet name="Sorted Array(Max to Min)" r:id="rId6" sheetId="4"/>
+    <sheet name="Sorted Array(Max to Min)" r:id="rId3" sheetId="1"/>
+    <sheet name="Sorted Array(Min to Max)" r:id="rId4" sheetId="2"/>
+    <sheet name="Sorted Array(Min to Max) + 1" r:id="rId5" sheetId="3"/>
+    <sheet name="Random Array" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
@@ -20,10 +20,10 @@
     <t>Length of array</t>
   </si>
   <si>
-    <t>Selection Sort</t>
+    <t>Bubble Sort (Down)</t>
   </si>
   <si>
-    <t>Bubble Sort (Down)</t>
+    <t>Selection Sort</t>
   </si>
   <si>
     <t>Bubble Sort (Up)</t>
@@ -84,7 +84,7 @@
           <a:bodyPr/>
           <a:p>
             <a:r>
-              <a:t>Random Array</a:t>
+              <a:t>Sorted Array(Max to Min)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -98,113 +98,113 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Selection Sort</c:v>
+            <c:v>Bubble Sort (Down)</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Random Array'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Max to Min)'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Random Array'!$B$2:$P$2</c:f>
+              <c:f>'Sorted Array(Max to Min)'!$B$2:$P$2</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>204661.0</c:v>
+                  <c:v>1.173935E7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>761896.0</c:v>
+                  <c:v>1.4864812E7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1867913.0</c:v>
+                  <c:v>1.3794415E7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6566674.0</c:v>
+                  <c:v>2.4524344E7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1601672.0</c:v>
+                  <c:v>5.4437498E7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>446150.0</c:v>
+                  <c:v>5.6255905E7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>836758.0</c:v>
+                  <c:v>7.6056738E7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1664459.0</c:v>
+                  <c:v>9.6285004E7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1498435.0</c:v>
+                  <c:v>1.36697466E8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1296189.0</c:v>
+                  <c:v>2.4198938E8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3049999.0</c:v>
+                  <c:v>2.2840325E8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2684748.0</c:v>
+                  <c:v>2.00752839E8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3242586.0</c:v>
+                  <c:v>2.29896855E8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1375277.0</c:v>
+                  <c:v>2.73516884E8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2525366.0</c:v>
+                  <c:v>3.15288322E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -214,113 +214,113 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Bubble Sort (Down)</c:v>
+            <c:v>Selection Sort</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Random Array'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Max to Min)'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Random Array'!$B$3:$P$3</c:f>
+              <c:f>'Sorted Array(Max to Min)'!$B$3:$P$3</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>501693.0</c:v>
+                  <c:v>6646361.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2018843.0</c:v>
+                  <c:v>6295600.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2472842.0</c:v>
+                  <c:v>5411752.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>781215.0</c:v>
+                  <c:v>2.280374E7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>553008.0</c:v>
+                  <c:v>5.5800096E7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>839172.0</c:v>
+                  <c:v>5.0219301E7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1037797.0</c:v>
+                  <c:v>7.2500219E7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1512925.0</c:v>
+                  <c:v>9.4825208E7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1566656.0</c:v>
+                  <c:v>1.54745094E8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1689211.0</c:v>
+                  <c:v>9.0536376E7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2677503.0</c:v>
+                  <c:v>9.5153632E7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2823603.0</c:v>
+                  <c:v>1.26187292E8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3598781.0</c:v>
+                  <c:v>8.9441226E7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3523920.0</c:v>
+                  <c:v>1.04578919E8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5640566.0</c:v>
+                  <c:v>1.21512683E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -337,106 +337,106 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Random Array'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Max to Min)'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Random Array'!$B$4:$P$4</c:f>
+              <c:f>'Sorted Array(Max to Min)'!$B$4:$P$4</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>313935.0</c:v>
+                  <c:v>8267955.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1342072.0</c:v>
+                  <c:v>1.2949809E7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3488301.0</c:v>
+                  <c:v>8623547.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1663856.0</c:v>
+                  <c:v>1.0673178E7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1692834.0</c:v>
+                  <c:v>1.4664376E7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1257551.0</c:v>
+                  <c:v>2.6956734E7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>886866.0</c:v>
+                  <c:v>4.2245358E7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1060738.0</c:v>
+                  <c:v>4.601982E7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1337846.0</c:v>
+                  <c:v>1.42840325E8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1651177.0</c:v>
+                  <c:v>8.0916086E7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1896288.0</c:v>
+                  <c:v>6.3475198E7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2216864.0</c:v>
+                  <c:v>7.693334E7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2298970.0</c:v>
+                  <c:v>1.10504438E8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3036113.0</c:v>
+                  <c:v>1.12524488E8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3477434.0</c:v>
+                  <c:v>1.2854301E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -453,106 +453,106 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Random Array'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Max to Min)'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Random Array'!$B$5:$P$5</c:f>
+              <c:f>'Sorted Array(Max to Min)'!$B$5:$P$5</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>601910.0</c:v>
+                  <c:v>2378056.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>620022.0</c:v>
+                  <c:v>3956182.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>287975.0</c:v>
+                  <c:v>2598414.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>396041.0</c:v>
+                  <c:v>1586579.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>658660.0</c:v>
+                  <c:v>2006767.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3253453.0</c:v>
+                  <c:v>4181370.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>745596.0</c:v>
+                  <c:v>1840745.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>750425.0</c:v>
+                  <c:v>1363805.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>801742.0</c:v>
+                  <c:v>6157951.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>979840.0</c:v>
+                  <c:v>2489744.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1050475.0</c:v>
+                  <c:v>1701285.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>597684.0</c:v>
+                  <c:v>1822633.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>681601.0</c:v>
+                  <c:v>4762753.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>687034.0</c:v>
+                  <c:v>2562794.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1213480.0</c:v>
+                  <c:v>2353303.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -569,106 +569,106 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Random Array'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Max to Min)'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Random Array'!$B$6:$P$6</c:f>
+              <c:f>'Sorted Array(Max to Min)'!$B$6:$P$6</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>379740.0</c:v>
+                  <c:v>538518.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68824.0</c:v>
+                  <c:v>299445.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>116518.0</c:v>
+                  <c:v>435887.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>103236.0</c:v>
+                  <c:v>575949.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>149723.0</c:v>
+                  <c:v>4877460.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>145497.0</c:v>
+                  <c:v>201039.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>151534.0</c:v>
+                  <c:v>190775.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>217339.0</c:v>
+                  <c:v>1270229.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>84521.0</c:v>
+                  <c:v>1.3755173E7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70031.0</c:v>
+                  <c:v>104444.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88747.0</c:v>
+                  <c:v>51316.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92369.0</c:v>
+                  <c:v>55542.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>90558.0</c:v>
+                  <c:v>112896.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>101425.0</c:v>
+                  <c:v>65202.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>97803.0</c:v>
+                  <c:v>68221.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -766,7 +766,7 @@
           <a:bodyPr/>
           <a:p>
             <a:r>
-              <a:t>Sorted Array(Min to Max) + 1</a:t>
+              <a:t>Sorted Array(Min to Max)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -780,113 +780,113 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Selection Sort</c:v>
+            <c:v>Bubble Sort (Down)</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Min to Max)'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>101.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>301.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>401.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>501.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>601.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>701.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>801.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>901.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1001.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1101.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1201.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1301.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1401.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1501.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$2:$P$2</c:f>
+              <c:f>'Sorted Array(Min to Max)'!$B$2:$P$2</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>12075.0</c:v>
+                  <c:v>649603.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33809.0</c:v>
+                  <c:v>2688368.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79692.0</c:v>
+                  <c:v>5936989.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>146101.0</c:v>
+                  <c:v>9839440.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>208888.0</c:v>
+                  <c:v>1.5543997E7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>313331.0</c:v>
+                  <c:v>2.4523739E7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>510748.0</c:v>
+                  <c:v>3.0672636E7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>536105.0</c:v>
+                  <c:v>3.866469E7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2676295.0</c:v>
+                  <c:v>6.3010332E7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1010026.0</c:v>
+                  <c:v>6.1191322E7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6628858.0</c:v>
+                  <c:v>8.1634514E7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1805730.0</c:v>
+                  <c:v>9.2994727E7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1748981.0</c:v>
+                  <c:v>1.27729799E8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7461993.0</c:v>
+                  <c:v>1.72617039E8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2148039.0</c:v>
+                  <c:v>1.70109183E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -896,113 +896,113 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Bubble Sort (Down)</c:v>
+            <c:v>Selection Sort</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Min to Max)'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>101.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>301.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>401.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>501.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>601.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>701.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>801.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>901.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1001.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1101.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1201.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1301.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1401.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1501.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$3:$P$3</c:f>
+              <c:f>'Sorted Array(Min to Max)'!$B$3:$P$3</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>12678.0</c:v>
+                  <c:v>537311.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41053.0</c:v>
+                  <c:v>1953641.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85728.0</c:v>
+                  <c:v>4580430.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>149119.0</c:v>
+                  <c:v>8538422.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>229414.0</c:v>
+                  <c:v>1.266908E7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>377326.0</c:v>
+                  <c:v>2.1723683E7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>754048.0</c:v>
+                  <c:v>2.6526885E7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>649000.0</c:v>
+                  <c:v>3.2920892E7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2093705.0</c:v>
+                  <c:v>6.0745173E7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1053493.0</c:v>
+                  <c:v>5.5435448E7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1266607.0</c:v>
+                  <c:v>6.6122513E7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1473683.0</c:v>
+                  <c:v>7.4109135E7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1550356.0</c:v>
+                  <c:v>1.36892469E8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2069556.0</c:v>
+                  <c:v>1.6079498E8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2425751.0</c:v>
+                  <c:v>1.57542736E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1019,106 +1019,106 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Min to Max)'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>101.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>301.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>401.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>501.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>601.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>701.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>801.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>901.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1001.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1101.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1201.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1301.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1401.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1501.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$4:$P$4</c:f>
+              <c:f>'Sorted Array(Min to Max)'!$B$4:$P$4</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8452.0</c:v>
+                  <c:v>1038400.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24752.0</c:v>
+                  <c:v>3157460.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44072.0</c:v>
+                  <c:v>7021272.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>73654.0</c:v>
+                  <c:v>1.2142635E7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>121952.0</c:v>
+                  <c:v>2.2859281E7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>169042.0</c:v>
+                  <c:v>2.9086058E7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>281334.0</c:v>
+                  <c:v>3.9188116E7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>273486.0</c:v>
+                  <c:v>5.4764715E7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>409323.0</c:v>
+                  <c:v>6.5694476E7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>465469.0</c:v>
+                  <c:v>8.2436254E7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>582590.0</c:v>
+                  <c:v>1.03958294E8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>687035.0</c:v>
+                  <c:v>1.21996867E8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>697298.0</c:v>
+                  <c:v>1.79230195E8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>884452.0</c:v>
+                  <c:v>2.0231708E8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1205631.0</c:v>
+                  <c:v>1.81992822E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1135,106 +1135,106 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Min to Max)'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>101.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>301.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>401.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>501.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>601.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>701.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>801.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>901.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1001.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1101.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1201.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1301.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1401.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1501.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$5:$P$5</c:f>
+              <c:f>'Sorted Array(Min to Max)'!$B$5:$P$5</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>35016.0</c:v>
+                  <c:v>240281.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60975.0</c:v>
+                  <c:v>310312.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85125.0</c:v>
+                  <c:v>418378.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>118329.0</c:v>
+                  <c:v>594665.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>149723.0</c:v>
+                  <c:v>826493.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>202850.0</c:v>
+                  <c:v>917052.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>218547.0</c:v>
+                  <c:v>994932.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>471506.0</c:v>
+                  <c:v>1568467.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>436491.0</c:v>
+                  <c:v>1466437.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>420190.0</c:v>
+                  <c:v>1491793.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>434076.0</c:v>
+                  <c:v>1965715.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>409323.0</c:v>
+                  <c:v>3144781.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>478751.0</c:v>
+                  <c:v>3060864.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>287975.0</c:v>
+                  <c:v>3652510.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>336876.0</c:v>
+                  <c:v>3042752.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1251,106 +1251,106 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Min to Max)'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>101.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>301.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>401.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>501.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>601.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>701.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>801.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>901.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1001.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1101.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1201.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1301.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1401.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1501.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max) + 1'!$B$6:$P$6</c:f>
+              <c:f>'Sorted Array(Min to Max)'!$B$6:$P$6</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>7245.0</c:v>
+                  <c:v>14489.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8452.0</c:v>
+                  <c:v>13885.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22338.0</c:v>
+                  <c:v>19923.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18716.0</c:v>
+                  <c:v>19319.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21130.0</c:v>
+                  <c:v>24752.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21130.0</c:v>
+                  <c:v>26563.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22942.0</c:v>
+                  <c:v>35620.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25356.0</c:v>
+                  <c:v>57957.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29582.0</c:v>
+                  <c:v>38035.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31997.0</c:v>
+                  <c:v>39846.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>80898.0</c:v>
+                  <c:v>43468.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>106858.0</c:v>
+                  <c:v>77276.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>99010.0</c:v>
+                  <c:v>84520.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>98407.0</c:v>
+                  <c:v>57957.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44072.0</c:v>
+                  <c:v>60976.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1448,7 +1448,7 @@
           <a:bodyPr/>
           <a:p>
             <a:r>
-              <a:t>Sorted Array(Min to Max)</a:t>
+              <a:t>Sorted Array(Min to Max) + 1</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1462,113 +1462,113 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Selection Sort</c:v>
+            <c:v>Bubble Sort (Down)</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1001.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2001.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3001.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4001.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5001.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6001.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7001.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8001.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9001.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10001.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11001.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12001.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13001.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14001.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15001.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$2:$P$2</c:f>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$2:$P$2</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>11471.0</c:v>
+                  <c:v>674960.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38638.0</c:v>
+                  <c:v>2704669.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100218.0</c:v>
+                  <c:v>5890503.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>158778.0</c:v>
+                  <c:v>1.0463084E7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>252356.0</c:v>
+                  <c:v>1.5727529E7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>359214.0</c:v>
+                  <c:v>2.5131687E7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>434075.0</c:v>
+                  <c:v>3.1648852E7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>597683.0</c:v>
+                  <c:v>3.9244262E7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>702128.0</c:v>
+                  <c:v>5.0551952E7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>827098.0</c:v>
+                  <c:v>6.5297227E7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1211668.0</c:v>
+                  <c:v>7.7050462E7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1463420.0</c:v>
+                  <c:v>9.3105812E7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1661440.0</c:v>
+                  <c:v>1.11592948E8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1727850.0</c:v>
+                  <c:v>1.24460651E8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2242824.0</c:v>
+                  <c:v>1.71327491E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1578,113 +1578,113 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Bubble Sort (Down)</c:v>
+            <c:v>Selection Sort</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1001.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2001.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3001.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4001.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5001.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6001.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7001.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8001.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9001.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10001.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11001.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12001.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13001.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14001.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15001.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$3:$P$3</c:f>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$3:$P$3</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>10867.0</c:v>
+                  <c:v>537915.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49505.0</c:v>
+                  <c:v>3404985.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>82106.0</c:v>
+                  <c:v>4908250.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>175683.0</c:v>
+                  <c:v>8648903.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>321180.0</c:v>
+                  <c:v>1.3937497E7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>390004.0</c:v>
+                  <c:v>2.9773695E7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>484184.0</c:v>
+                  <c:v>2.7072045E7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>604324.0</c:v>
+                  <c:v>3.4265982E7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>763708.0</c:v>
+                  <c:v>4.676783E7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>942409.0</c:v>
+                  <c:v>5.3691903E7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1588994.0</c:v>
+                  <c:v>6.4578195E7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1566052.0</c:v>
+                  <c:v>7.6851838E7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2542269.0</c:v>
+                  <c:v>8.8228351E7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1841349.0</c:v>
+                  <c:v>1.26554958E8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2158302.0</c:v>
+                  <c:v>1.75539651E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1701,106 +1701,106 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1001.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2001.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3001.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4001.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5001.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6001.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7001.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8001.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9001.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10001.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11001.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12001.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13001.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14001.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15001.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$4:$P$4</c:f>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$4:$P$4</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>6641.0</c:v>
+                  <c:v>808382.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19319.0</c:v>
+                  <c:v>3098899.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44072.0</c:v>
+                  <c:v>6579952.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76672.0</c:v>
+                  <c:v>1.341709E7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>119537.0</c:v>
+                  <c:v>2.1487025E7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>186550.0</c:v>
+                  <c:v>2.8006605E7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>220962.0</c:v>
+                  <c:v>4.0900873E7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>319369.0</c:v>
+                  <c:v>5.2917933E7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>356799.0</c:v>
+                  <c:v>6.7700035E7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>517993.0</c:v>
+                  <c:v>8.0648034E7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>511351.0</c:v>
+                  <c:v>9.9562E7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>648396.0</c:v>
+                  <c:v>1.20064357E8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>784838.0</c:v>
+                  <c:v>1.31465019E8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>660471.0</c:v>
+                  <c:v>1.6640113E8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>933956.0</c:v>
+                  <c:v>1.85073005E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1817,106 +1817,106 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1001.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2001.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3001.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4001.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5001.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6001.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7001.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8001.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9001.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10001.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11001.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12001.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13001.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14001.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15001.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$5:$P$5</c:f>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$5:$P$5</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>22941.0</c:v>
+                  <c:v>212510.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41053.0</c:v>
+                  <c:v>268052.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61579.0</c:v>
+                  <c:v>497465.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>83313.0</c:v>
+                  <c:v>554819.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>103237.0</c:v>
+                  <c:v>1173030.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>121952.0</c:v>
+                  <c:v>854869.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>154552.0</c:v>
+                  <c:v>1235213.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>165420.0</c:v>
+                  <c:v>1391577.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>188361.0</c:v>
+                  <c:v>1389765.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>222773.0</c:v>
+                  <c:v>1837726.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>263826.0</c:v>
+                  <c:v>1688607.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>256581.0</c:v>
+                  <c:v>2098533.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>275297.0</c:v>
+                  <c:v>2631619.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>207680.0</c:v>
+                  <c:v>3528748.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>323595.0</c:v>
+                  <c:v>3292693.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1933,106 +1933,106 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$1:$P$1</c:f>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1001.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2001.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3001.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4001.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5001.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6001.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7001.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8001.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9001.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10001.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11001.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12001.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13001.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14001.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15001.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Min to Max)'!$B$6:$P$6</c:f>
+              <c:f>'Sorted Array(Min to Max) + 1'!$B$6:$P$6</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>4226.0</c:v>
+                  <c:v>12075.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7848.0</c:v>
+                  <c:v>13886.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15093.0</c:v>
+                  <c:v>16301.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16301.0</c:v>
+                  <c:v>20527.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18716.0</c:v>
+                  <c:v>37431.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21131.0</c:v>
+                  <c:v>27167.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24148.0</c:v>
+                  <c:v>31997.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50712.0</c:v>
+                  <c:v>35619.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28375.0</c:v>
+                  <c:v>36223.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30790.0</c:v>
+                  <c:v>43468.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>156968.0</c:v>
+                  <c:v>58561.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36827.0</c:v>
+                  <c:v>50713.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>55542.0</c:v>
+                  <c:v>51316.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>46486.0</c:v>
+                  <c:v>63995.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43468.0</c:v>
+                  <c:v>82709.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2130,7 +2130,7 @@
           <a:bodyPr/>
           <a:p>
             <a:r>
-              <a:t>Sorted Array(Max to Min)</a:t>
+              <a:t>Random Array</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2144,113 +2144,113 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Selection Sort</c:v>
+            <c:v>Bubble Sort (Down)</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$1:$P$1</c:f>
+              <c:f>'Random Array'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$2:$P$2</c:f>
+              <c:f>'Random Array'!$B$2:$P$2</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>13282.0</c:v>
+                  <c:v>1939151.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53128.0</c:v>
+                  <c:v>6902943.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>91766.0</c:v>
+                  <c:v>1.2691417E7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1489984.0</c:v>
+                  <c:v>2.4389714E7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>543952.0</c:v>
+                  <c:v>4.0407633E7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1313093.0</c:v>
+                  <c:v>6.1989441E7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>489014.0</c:v>
+                  <c:v>9.0489285E7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>650207.0</c:v>
+                  <c:v>1.20439871E8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1333016.0</c:v>
+                  <c:v>1.4930557E8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1259362.0</c:v>
+                  <c:v>2.27620223E8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1221328.0</c:v>
+                  <c:v>2.41519082E8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1327582.0</c:v>
+                  <c:v>2.92253961E8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1520773.0</c:v>
+                  <c:v>3.54339393E8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1647555.0</c:v>
+                  <c:v>5.13628694E8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1239439.0</c:v>
+                  <c:v>6.43312737E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2260,113 +2260,113 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Bubble Sort (Down)</c:v>
+            <c:v>Selection Sort</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$1:$P$1</c:f>
+              <c:f>'Random Array'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$3:$P$3</c:f>
+              <c:f>'Random Array'!$B$3:$P$3</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>24752.0</c:v>
+                  <c:v>600702.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>159382.0</c:v>
+                  <c:v>4129450.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200436.0</c:v>
+                  <c:v>4979489.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>301257.0</c:v>
+                  <c:v>1.3048216E7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>453998.0</c:v>
+                  <c:v>1.482557E7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2394357.0</c:v>
+                  <c:v>1.9929425E7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>955690.0</c:v>
+                  <c:v>2.7543551E7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1255740.0</c:v>
+                  <c:v>3.9020282E7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1452553.0</c:v>
+                  <c:v>4.4323365E7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.059836E7</c:v>
+                  <c:v>5.5433034E7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7913576.0</c:v>
+                  <c:v>7.11829E7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2404018.0</c:v>
+                  <c:v>7.3801237E7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3621723.0</c:v>
+                  <c:v>1.05738064E8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3109163.0</c:v>
+                  <c:v>1.12300508E8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5793308.0</c:v>
+                  <c:v>1.73700114E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2383,106 +2383,106 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$1:$P$1</c:f>
+              <c:f>'Random Array'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$4:$P$4</c:f>
+              <c:f>'Random Array'!$B$4:$P$4</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>14490.0</c:v>
+                  <c:v>1805729.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>172664.0</c:v>
+                  <c:v>5299461.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95991.0</c:v>
+                  <c:v>1.1910202E7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>143685.0</c:v>
+                  <c:v>2.4334171E7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>542142.0</c:v>
+                  <c:v>4.0091283E7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>321180.0</c:v>
+                  <c:v>5.9855289E7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>485392.0</c:v>
+                  <c:v>8.059551E7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>557235.0</c:v>
+                  <c:v>1.12750883E8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>773971.0</c:v>
+                  <c:v>1.47025921E8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>957502.0</c:v>
+                  <c:v>1.83634338E8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1063152.0</c:v>
+                  <c:v>2.7331162E8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1222535.0</c:v>
+                  <c:v>2.90265909E8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1301623.0</c:v>
+                  <c:v>3.43838275E8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1191141.0</c:v>
+                  <c:v>3.9375632E8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3051810.0</c:v>
+                  <c:v>5.59637044E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2499,106 +2499,106 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$1:$P$1</c:f>
+              <c:f>'Random Array'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$5:$P$5</c:f>
+              <c:f>'Random Array'!$B$5:$P$5</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>21130.0</c:v>
+                  <c:v>281333.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44675.0</c:v>
+                  <c:v>342913.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95388.0</c:v>
+                  <c:v>549385.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84521.0</c:v>
+                  <c:v>554820.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>109877.0</c:v>
+                  <c:v>649604.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>145496.0</c:v>
+                  <c:v>728087.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>193795.0</c:v>
+                  <c:v>898337.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>185946.0</c:v>
+                  <c:v>1427800.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>202851.0</c:v>
+                  <c:v>1214686.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>204662.0</c:v>
+                  <c:v>1237023.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>245111.0</c:v>
+                  <c:v>1778561.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>268052.0</c:v>
+                  <c:v>1738716.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>285560.0</c:v>
+                  <c:v>1832896.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>237866.0</c:v>
+                  <c:v>1942774.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>353781.0</c:v>
+                  <c:v>2448691.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2615,106 +2615,106 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$1:$P$1</c:f>
+              <c:f>'Random Array'!$B$1:$P$1</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200.0</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300.0</c:v>
+                  <c:v>3000.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>4000.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500.0</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>6000.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>700.0</c:v>
+                  <c:v>7000.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>800.0</c:v>
+                  <c:v>8000.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>900.0</c:v>
+                  <c:v>9000.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000.0</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1100.0</c:v>
+                  <c:v>11000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1200.0</c:v>
+                  <c:v>12000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300.0</c:v>
+                  <c:v>13000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1400.0</c:v>
+                  <c:v>14000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1500.0</c:v>
+                  <c:v>15000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sorted Array(Max to Min)'!$B$6:$P$6</c:f>
+              <c:f>'Random Array'!$B$6:$P$6</c:f>
               <c:numCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>13885.0</c:v>
+                  <c:v>51316.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10867.0</c:v>
+                  <c:v>56750.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19319.0</c:v>
+                  <c:v>78484.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>205869.0</c:v>
+                  <c:v>93576.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24149.0</c:v>
+                  <c:v>115311.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>96595.0</c:v>
+                  <c:v>120141.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27772.0</c:v>
+                  <c:v>148516.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29582.0</c:v>
+                  <c:v>167834.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36224.0</c:v>
+                  <c:v>223981.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38034.0</c:v>
+                  <c:v>184739.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18112.0</c:v>
+                  <c:v>194398.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17508.0</c:v>
+                  <c:v>228207.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16904.0</c:v>
+                  <c:v>272278.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13282.0</c:v>
+                  <c:v>251148.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19922.0</c:v>
+                  <c:v>298841.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2959,49 +2959,49 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>100.0</v>
+        <v>1000.0</v>
       </c>
       <c r="C1" t="n">
-        <v>200.0</v>
+        <v>2000.0</v>
       </c>
       <c r="D1" t="n">
-        <v>300.0</v>
+        <v>3000.0</v>
       </c>
       <c r="E1" t="n">
-        <v>400.0</v>
+        <v>4000.0</v>
       </c>
       <c r="F1" t="n">
-        <v>500.0</v>
+        <v>5000.0</v>
       </c>
       <c r="G1" t="n">
-        <v>600.0</v>
+        <v>6000.0</v>
       </c>
       <c r="H1" t="n">
-        <v>700.0</v>
+        <v>7000.0</v>
       </c>
       <c r="I1" t="n">
-        <v>800.0</v>
+        <v>8000.0</v>
       </c>
       <c r="J1" t="n">
-        <v>900.0</v>
+        <v>9000.0</v>
       </c>
       <c r="K1" t="n">
-        <v>1000.0</v>
+        <v>10000.0</v>
       </c>
       <c r="L1" t="n">
-        <v>1100.0</v>
+        <v>11000.0</v>
       </c>
       <c r="M1" t="n">
-        <v>1200.0</v>
+        <v>12000.0</v>
       </c>
       <c r="N1" t="n">
-        <v>1300.0</v>
+        <v>13000.0</v>
       </c>
       <c r="O1" t="n">
-        <v>1400.0</v>
+        <v>14000.0</v>
       </c>
       <c r="P1" t="n">
-        <v>1500.0</v>
+        <v>15000.0</v>
       </c>
     </row>
     <row r="2">
@@ -3009,49 +3009,49 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>204661.0</v>
+        <v>1.173935E7</v>
       </c>
       <c r="C2" t="n">
-        <v>761896.0</v>
+        <v>1.4864812E7</v>
       </c>
       <c r="D2" t="n">
-        <v>1867913.0</v>
+        <v>1.3794415E7</v>
       </c>
       <c r="E2" t="n">
-        <v>6566674.0</v>
+        <v>2.4524344E7</v>
       </c>
       <c r="F2" t="n">
-        <v>1601672.0</v>
+        <v>5.4437498E7</v>
       </c>
       <c r="G2" t="n">
-        <v>446150.0</v>
+        <v>5.6255905E7</v>
       </c>
       <c r="H2" t="n">
-        <v>836758.0</v>
+        <v>7.6056738E7</v>
       </c>
       <c r="I2" t="n">
-        <v>1664459.0</v>
+        <v>9.6285004E7</v>
       </c>
       <c r="J2" t="n">
-        <v>1498435.0</v>
+        <v>1.36697466E8</v>
       </c>
       <c r="K2" t="n">
-        <v>1296189.0</v>
+        <v>2.4198938E8</v>
       </c>
       <c r="L2" t="n">
-        <v>3049999.0</v>
+        <v>2.2840325E8</v>
       </c>
       <c r="M2" t="n">
-        <v>2684748.0</v>
+        <v>2.00752839E8</v>
       </c>
       <c r="N2" t="n">
-        <v>3242586.0</v>
+        <v>2.29896855E8</v>
       </c>
       <c r="O2" t="n">
-        <v>1375277.0</v>
+        <v>2.73516884E8</v>
       </c>
       <c r="P2" t="n">
-        <v>2525366.0</v>
+        <v>3.15288322E8</v>
       </c>
     </row>
     <row r="3">
@@ -3059,49 +3059,49 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>501693.0</v>
+        <v>6646361.0</v>
       </c>
       <c r="C3" t="n">
-        <v>2018843.0</v>
+        <v>6295600.0</v>
       </c>
       <c r="D3" t="n">
-        <v>2472842.0</v>
+        <v>5411752.0</v>
       </c>
       <c r="E3" t="n">
-        <v>781215.0</v>
+        <v>2.280374E7</v>
       </c>
       <c r="F3" t="n">
-        <v>553008.0</v>
+        <v>5.5800096E7</v>
       </c>
       <c r="G3" t="n">
-        <v>839172.0</v>
+        <v>5.0219301E7</v>
       </c>
       <c r="H3" t="n">
-        <v>1037797.0</v>
+        <v>7.2500219E7</v>
       </c>
       <c r="I3" t="n">
-        <v>1512925.0</v>
+        <v>9.4825208E7</v>
       </c>
       <c r="J3" t="n">
-        <v>1566656.0</v>
+        <v>1.54745094E8</v>
       </c>
       <c r="K3" t="n">
-        <v>1689211.0</v>
+        <v>9.0536376E7</v>
       </c>
       <c r="L3" t="n">
-        <v>2677503.0</v>
+        <v>9.5153632E7</v>
       </c>
       <c r="M3" t="n">
-        <v>2823603.0</v>
+        <v>1.26187292E8</v>
       </c>
       <c r="N3" t="n">
-        <v>3598781.0</v>
+        <v>8.9441226E7</v>
       </c>
       <c r="O3" t="n">
-        <v>3523920.0</v>
+        <v>1.04578919E8</v>
       </c>
       <c r="P3" t="n">
-        <v>5640566.0</v>
+        <v>1.21512683E8</v>
       </c>
     </row>
     <row r="4">
@@ -3109,49 +3109,49 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>313935.0</v>
+        <v>8267955.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1342072.0</v>
+        <v>1.2949809E7</v>
       </c>
       <c r="D4" t="n">
-        <v>3488301.0</v>
+        <v>8623547.0</v>
       </c>
       <c r="E4" t="n">
-        <v>1663856.0</v>
+        <v>1.0673178E7</v>
       </c>
       <c r="F4" t="n">
-        <v>1692834.0</v>
+        <v>1.4664376E7</v>
       </c>
       <c r="G4" t="n">
-        <v>1257551.0</v>
+        <v>2.6956734E7</v>
       </c>
       <c r="H4" t="n">
-        <v>886866.0</v>
+        <v>4.2245358E7</v>
       </c>
       <c r="I4" t="n">
-        <v>1060738.0</v>
+        <v>4.601982E7</v>
       </c>
       <c r="J4" t="n">
-        <v>1337846.0</v>
+        <v>1.42840325E8</v>
       </c>
       <c r="K4" t="n">
-        <v>1651177.0</v>
+        <v>8.0916086E7</v>
       </c>
       <c r="L4" t="n">
-        <v>1896288.0</v>
+        <v>6.3475198E7</v>
       </c>
       <c r="M4" t="n">
-        <v>2216864.0</v>
+        <v>7.693334E7</v>
       </c>
       <c r="N4" t="n">
-        <v>2298970.0</v>
+        <v>1.10504438E8</v>
       </c>
       <c r="O4" t="n">
-        <v>3036113.0</v>
+        <v>1.12524488E8</v>
       </c>
       <c r="P4" t="n">
-        <v>3477434.0</v>
+        <v>1.2854301E8</v>
       </c>
     </row>
     <row r="5">
@@ -3159,49 +3159,49 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>601910.0</v>
+        <v>2378056.0</v>
       </c>
       <c r="C5" t="n">
-        <v>620022.0</v>
+        <v>3956182.0</v>
       </c>
       <c r="D5" t="n">
-        <v>287975.0</v>
+        <v>2598414.0</v>
       </c>
       <c r="E5" t="n">
-        <v>396041.0</v>
+        <v>1586579.0</v>
       </c>
       <c r="F5" t="n">
-        <v>658660.0</v>
+        <v>2006767.0</v>
       </c>
       <c r="G5" t="n">
-        <v>3253453.0</v>
+        <v>4181370.0</v>
       </c>
       <c r="H5" t="n">
-        <v>745596.0</v>
+        <v>1840745.0</v>
       </c>
       <c r="I5" t="n">
-        <v>750425.0</v>
+        <v>1363805.0</v>
       </c>
       <c r="J5" t="n">
-        <v>801742.0</v>
+        <v>6157951.0</v>
       </c>
       <c r="K5" t="n">
-        <v>979840.0</v>
+        <v>2489744.0</v>
       </c>
       <c r="L5" t="n">
-        <v>1050475.0</v>
+        <v>1701285.0</v>
       </c>
       <c r="M5" t="n">
-        <v>597684.0</v>
+        <v>1822633.0</v>
       </c>
       <c r="N5" t="n">
-        <v>681601.0</v>
+        <v>4762753.0</v>
       </c>
       <c r="O5" t="n">
-        <v>687034.0</v>
+        <v>2562794.0</v>
       </c>
       <c r="P5" t="n">
-        <v>1213480.0</v>
+        <v>2353303.0</v>
       </c>
     </row>
     <row r="6">
@@ -3209,49 +3209,49 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>379740.0</v>
+        <v>538518.0</v>
       </c>
       <c r="C6" t="n">
-        <v>68824.0</v>
+        <v>299445.0</v>
       </c>
       <c r="D6" t="n">
-        <v>116518.0</v>
+        <v>435887.0</v>
       </c>
       <c r="E6" t="n">
-        <v>103236.0</v>
+        <v>575949.0</v>
       </c>
       <c r="F6" t="n">
-        <v>149723.0</v>
+        <v>4877460.0</v>
       </c>
       <c r="G6" t="n">
-        <v>145497.0</v>
+        <v>201039.0</v>
       </c>
       <c r="H6" t="n">
-        <v>151534.0</v>
+        <v>190775.0</v>
       </c>
       <c r="I6" t="n">
-        <v>217339.0</v>
+        <v>1270229.0</v>
       </c>
       <c r="J6" t="n">
-        <v>84521.0</v>
+        <v>1.3755173E7</v>
       </c>
       <c r="K6" t="n">
-        <v>70031.0</v>
+        <v>104444.0</v>
       </c>
       <c r="L6" t="n">
-        <v>88747.0</v>
+        <v>51316.0</v>
       </c>
       <c r="M6" t="n">
-        <v>92369.0</v>
+        <v>55542.0</v>
       </c>
       <c r="N6" t="n">
-        <v>90558.0</v>
+        <v>112896.0</v>
       </c>
       <c r="O6" t="n">
-        <v>101425.0</v>
+        <v>65202.0</v>
       </c>
       <c r="P6" t="n">
-        <v>97803.0</v>
+        <v>68221.0</v>
       </c>
     </row>
   </sheetData>
@@ -3276,49 +3276,49 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>101.0</v>
+        <v>1000.0</v>
       </c>
       <c r="C1" t="n">
-        <v>201.0</v>
+        <v>2000.0</v>
       </c>
       <c r="D1" t="n">
-        <v>301.0</v>
+        <v>3000.0</v>
       </c>
       <c r="E1" t="n">
-        <v>401.0</v>
+        <v>4000.0</v>
       </c>
       <c r="F1" t="n">
-        <v>501.0</v>
+        <v>5000.0</v>
       </c>
       <c r="G1" t="n">
-        <v>601.0</v>
+        <v>6000.0</v>
       </c>
       <c r="H1" t="n">
-        <v>701.0</v>
+        <v>7000.0</v>
       </c>
       <c r="I1" t="n">
-        <v>801.0</v>
+        <v>8000.0</v>
       </c>
       <c r="J1" t="n">
-        <v>901.0</v>
+        <v>9000.0</v>
       </c>
       <c r="K1" t="n">
-        <v>1001.0</v>
+        <v>10000.0</v>
       </c>
       <c r="L1" t="n">
-        <v>1101.0</v>
+        <v>11000.0</v>
       </c>
       <c r="M1" t="n">
-        <v>1201.0</v>
+        <v>12000.0</v>
       </c>
       <c r="N1" t="n">
-        <v>1301.0</v>
+        <v>13000.0</v>
       </c>
       <c r="O1" t="n">
-        <v>1401.0</v>
+        <v>14000.0</v>
       </c>
       <c r="P1" t="n">
-        <v>1501.0</v>
+        <v>15000.0</v>
       </c>
     </row>
     <row r="2">
@@ -3326,49 +3326,49 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>12075.0</v>
+        <v>649603.0</v>
       </c>
       <c r="C2" t="n">
-        <v>33809.0</v>
+        <v>2688368.0</v>
       </c>
       <c r="D2" t="n">
-        <v>79692.0</v>
+        <v>5936989.0</v>
       </c>
       <c r="E2" t="n">
-        <v>146101.0</v>
+        <v>9839440.0</v>
       </c>
       <c r="F2" t="n">
-        <v>208888.0</v>
+        <v>1.5543997E7</v>
       </c>
       <c r="G2" t="n">
-        <v>313331.0</v>
+        <v>2.4523739E7</v>
       </c>
       <c r="H2" t="n">
-        <v>510748.0</v>
+        <v>3.0672636E7</v>
       </c>
       <c r="I2" t="n">
-        <v>536105.0</v>
+        <v>3.866469E7</v>
       </c>
       <c r="J2" t="n">
-        <v>2676295.0</v>
+        <v>6.3010332E7</v>
       </c>
       <c r="K2" t="n">
-        <v>1010026.0</v>
+        <v>6.1191322E7</v>
       </c>
       <c r="L2" t="n">
-        <v>6628858.0</v>
+        <v>8.1634514E7</v>
       </c>
       <c r="M2" t="n">
-        <v>1805730.0</v>
+        <v>9.2994727E7</v>
       </c>
       <c r="N2" t="n">
-        <v>1748981.0</v>
+        <v>1.27729799E8</v>
       </c>
       <c r="O2" t="n">
-        <v>7461993.0</v>
+        <v>1.72617039E8</v>
       </c>
       <c r="P2" t="n">
-        <v>2148039.0</v>
+        <v>1.70109183E8</v>
       </c>
     </row>
     <row r="3">
@@ -3376,49 +3376,49 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>12678.0</v>
+        <v>537311.0</v>
       </c>
       <c r="C3" t="n">
-        <v>41053.0</v>
+        <v>1953641.0</v>
       </c>
       <c r="D3" t="n">
-        <v>85728.0</v>
+        <v>4580430.0</v>
       </c>
       <c r="E3" t="n">
-        <v>149119.0</v>
+        <v>8538422.0</v>
       </c>
       <c r="F3" t="n">
-        <v>229414.0</v>
+        <v>1.266908E7</v>
       </c>
       <c r="G3" t="n">
-        <v>377326.0</v>
+        <v>2.1723683E7</v>
       </c>
       <c r="H3" t="n">
-        <v>754048.0</v>
+        <v>2.6526885E7</v>
       </c>
       <c r="I3" t="n">
-        <v>649000.0</v>
+        <v>3.2920892E7</v>
       </c>
       <c r="J3" t="n">
-        <v>2093705.0</v>
+        <v>6.0745173E7</v>
       </c>
       <c r="K3" t="n">
-        <v>1053493.0</v>
+        <v>5.5435448E7</v>
       </c>
       <c r="L3" t="n">
-        <v>1266607.0</v>
+        <v>6.6122513E7</v>
       </c>
       <c r="M3" t="n">
-        <v>1473683.0</v>
+        <v>7.4109135E7</v>
       </c>
       <c r="N3" t="n">
-        <v>1550356.0</v>
+        <v>1.36892469E8</v>
       </c>
       <c r="O3" t="n">
-        <v>2069556.0</v>
+        <v>1.6079498E8</v>
       </c>
       <c r="P3" t="n">
-        <v>2425751.0</v>
+        <v>1.57542736E8</v>
       </c>
     </row>
     <row r="4">
@@ -3426,49 +3426,49 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>8452.0</v>
+        <v>1038400.0</v>
       </c>
       <c r="C4" t="n">
-        <v>24752.0</v>
+        <v>3157460.0</v>
       </c>
       <c r="D4" t="n">
-        <v>44072.0</v>
+        <v>7021272.0</v>
       </c>
       <c r="E4" t="n">
-        <v>73654.0</v>
+        <v>1.2142635E7</v>
       </c>
       <c r="F4" t="n">
-        <v>121952.0</v>
+        <v>2.2859281E7</v>
       </c>
       <c r="G4" t="n">
-        <v>169042.0</v>
+        <v>2.9086058E7</v>
       </c>
       <c r="H4" t="n">
-        <v>281334.0</v>
+        <v>3.9188116E7</v>
       </c>
       <c r="I4" t="n">
-        <v>273486.0</v>
+        <v>5.4764715E7</v>
       </c>
       <c r="J4" t="n">
-        <v>409323.0</v>
+        <v>6.5694476E7</v>
       </c>
       <c r="K4" t="n">
-        <v>465469.0</v>
+        <v>8.2436254E7</v>
       </c>
       <c r="L4" t="n">
-        <v>582590.0</v>
+        <v>1.03958294E8</v>
       </c>
       <c r="M4" t="n">
-        <v>687035.0</v>
+        <v>1.21996867E8</v>
       </c>
       <c r="N4" t="n">
-        <v>697298.0</v>
+        <v>1.79230195E8</v>
       </c>
       <c r="O4" t="n">
-        <v>884452.0</v>
+        <v>2.0231708E8</v>
       </c>
       <c r="P4" t="n">
-        <v>1205631.0</v>
+        <v>1.81992822E8</v>
       </c>
     </row>
     <row r="5">
@@ -3476,49 +3476,49 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>35016.0</v>
+        <v>240281.0</v>
       </c>
       <c r="C5" t="n">
-        <v>60975.0</v>
+        <v>310312.0</v>
       </c>
       <c r="D5" t="n">
-        <v>85125.0</v>
+        <v>418378.0</v>
       </c>
       <c r="E5" t="n">
-        <v>118329.0</v>
+        <v>594665.0</v>
       </c>
       <c r="F5" t="n">
-        <v>149723.0</v>
+        <v>826493.0</v>
       </c>
       <c r="G5" t="n">
-        <v>202850.0</v>
+        <v>917052.0</v>
       </c>
       <c r="H5" t="n">
-        <v>218547.0</v>
+        <v>994932.0</v>
       </c>
       <c r="I5" t="n">
-        <v>471506.0</v>
+        <v>1568467.0</v>
       </c>
       <c r="J5" t="n">
-        <v>436491.0</v>
+        <v>1466437.0</v>
       </c>
       <c r="K5" t="n">
-        <v>420190.0</v>
+        <v>1491793.0</v>
       </c>
       <c r="L5" t="n">
-        <v>434076.0</v>
+        <v>1965715.0</v>
       </c>
       <c r="M5" t="n">
-        <v>409323.0</v>
+        <v>3144781.0</v>
       </c>
       <c r="N5" t="n">
-        <v>478751.0</v>
+        <v>3060864.0</v>
       </c>
       <c r="O5" t="n">
-        <v>287975.0</v>
+        <v>3652510.0</v>
       </c>
       <c r="P5" t="n">
-        <v>336876.0</v>
+        <v>3042752.0</v>
       </c>
     </row>
     <row r="6">
@@ -3526,49 +3526,49 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>7245.0</v>
+        <v>14489.0</v>
       </c>
       <c r="C6" t="n">
-        <v>8452.0</v>
+        <v>13885.0</v>
       </c>
       <c r="D6" t="n">
-        <v>22338.0</v>
+        <v>19923.0</v>
       </c>
       <c r="E6" t="n">
-        <v>18716.0</v>
+        <v>19319.0</v>
       </c>
       <c r="F6" t="n">
-        <v>21130.0</v>
+        <v>24752.0</v>
       </c>
       <c r="G6" t="n">
-        <v>21130.0</v>
+        <v>26563.0</v>
       </c>
       <c r="H6" t="n">
-        <v>22942.0</v>
+        <v>35620.0</v>
       </c>
       <c r="I6" t="n">
-        <v>25356.0</v>
+        <v>57957.0</v>
       </c>
       <c r="J6" t="n">
-        <v>29582.0</v>
+        <v>38035.0</v>
       </c>
       <c r="K6" t="n">
-        <v>31997.0</v>
+        <v>39846.0</v>
       </c>
       <c r="L6" t="n">
-        <v>80898.0</v>
+        <v>43468.0</v>
       </c>
       <c r="M6" t="n">
-        <v>106858.0</v>
+        <v>77276.0</v>
       </c>
       <c r="N6" t="n">
-        <v>99010.0</v>
+        <v>84520.0</v>
       </c>
       <c r="O6" t="n">
-        <v>98407.0</v>
+        <v>57957.0</v>
       </c>
       <c r="P6" t="n">
-        <v>44072.0</v>
+        <v>60976.0</v>
       </c>
     </row>
   </sheetData>
@@ -3593,49 +3593,49 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>100.0</v>
+        <v>1001.0</v>
       </c>
       <c r="C1" t="n">
-        <v>200.0</v>
+        <v>2001.0</v>
       </c>
       <c r="D1" t="n">
-        <v>300.0</v>
+        <v>3001.0</v>
       </c>
       <c r="E1" t="n">
-        <v>400.0</v>
+        <v>4001.0</v>
       </c>
       <c r="F1" t="n">
-        <v>500.0</v>
+        <v>5001.0</v>
       </c>
       <c r="G1" t="n">
-        <v>600.0</v>
+        <v>6001.0</v>
       </c>
       <c r="H1" t="n">
-        <v>700.0</v>
+        <v>7001.0</v>
       </c>
       <c r="I1" t="n">
-        <v>800.0</v>
+        <v>8001.0</v>
       </c>
       <c r="J1" t="n">
-        <v>900.0</v>
+        <v>9001.0</v>
       </c>
       <c r="K1" t="n">
-        <v>1000.0</v>
+        <v>10001.0</v>
       </c>
       <c r="L1" t="n">
-        <v>1100.0</v>
+        <v>11001.0</v>
       </c>
       <c r="M1" t="n">
-        <v>1200.0</v>
+        <v>12001.0</v>
       </c>
       <c r="N1" t="n">
-        <v>1300.0</v>
+        <v>13001.0</v>
       </c>
       <c r="O1" t="n">
-        <v>1400.0</v>
+        <v>14001.0</v>
       </c>
       <c r="P1" t="n">
-        <v>1500.0</v>
+        <v>15001.0</v>
       </c>
     </row>
     <row r="2">
@@ -3643,49 +3643,49 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>11471.0</v>
+        <v>674960.0</v>
       </c>
       <c r="C2" t="n">
-        <v>38638.0</v>
+        <v>2704669.0</v>
       </c>
       <c r="D2" t="n">
-        <v>100218.0</v>
+        <v>5890503.0</v>
       </c>
       <c r="E2" t="n">
-        <v>158778.0</v>
+        <v>1.0463084E7</v>
       </c>
       <c r="F2" t="n">
-        <v>252356.0</v>
+        <v>1.5727529E7</v>
       </c>
       <c r="G2" t="n">
-        <v>359214.0</v>
+        <v>2.5131687E7</v>
       </c>
       <c r="H2" t="n">
-        <v>434075.0</v>
+        <v>3.1648852E7</v>
       </c>
       <c r="I2" t="n">
-        <v>597683.0</v>
+        <v>3.9244262E7</v>
       </c>
       <c r="J2" t="n">
-        <v>702128.0</v>
+        <v>5.0551952E7</v>
       </c>
       <c r="K2" t="n">
-        <v>827098.0</v>
+        <v>6.5297227E7</v>
       </c>
       <c r="L2" t="n">
-        <v>1211668.0</v>
+        <v>7.7050462E7</v>
       </c>
       <c r="M2" t="n">
-        <v>1463420.0</v>
+        <v>9.3105812E7</v>
       </c>
       <c r="N2" t="n">
-        <v>1661440.0</v>
+        <v>1.11592948E8</v>
       </c>
       <c r="O2" t="n">
-        <v>1727850.0</v>
+        <v>1.24460651E8</v>
       </c>
       <c r="P2" t="n">
-        <v>2242824.0</v>
+        <v>1.71327491E8</v>
       </c>
     </row>
     <row r="3">
@@ -3693,49 +3693,49 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>10867.0</v>
+        <v>537915.0</v>
       </c>
       <c r="C3" t="n">
-        <v>49505.0</v>
+        <v>3404985.0</v>
       </c>
       <c r="D3" t="n">
-        <v>82106.0</v>
+        <v>4908250.0</v>
       </c>
       <c r="E3" t="n">
-        <v>175683.0</v>
+        <v>8648903.0</v>
       </c>
       <c r="F3" t="n">
-        <v>321180.0</v>
+        <v>1.3937497E7</v>
       </c>
       <c r="G3" t="n">
-        <v>390004.0</v>
+        <v>2.9773695E7</v>
       </c>
       <c r="H3" t="n">
-        <v>484184.0</v>
+        <v>2.7072045E7</v>
       </c>
       <c r="I3" t="n">
-        <v>604324.0</v>
+        <v>3.4265982E7</v>
       </c>
       <c r="J3" t="n">
-        <v>763708.0</v>
+        <v>4.676783E7</v>
       </c>
       <c r="K3" t="n">
-        <v>942409.0</v>
+        <v>5.3691903E7</v>
       </c>
       <c r="L3" t="n">
-        <v>1588994.0</v>
+        <v>6.4578195E7</v>
       </c>
       <c r="M3" t="n">
-        <v>1566052.0</v>
+        <v>7.6851838E7</v>
       </c>
       <c r="N3" t="n">
-        <v>2542269.0</v>
+        <v>8.8228351E7</v>
       </c>
       <c r="O3" t="n">
-        <v>1841349.0</v>
+        <v>1.26554958E8</v>
       </c>
       <c r="P3" t="n">
-        <v>2158302.0</v>
+        <v>1.75539651E8</v>
       </c>
     </row>
     <row r="4">
@@ -3743,49 +3743,49 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>6641.0</v>
+        <v>808382.0</v>
       </c>
       <c r="C4" t="n">
-        <v>19319.0</v>
+        <v>3098899.0</v>
       </c>
       <c r="D4" t="n">
-        <v>44072.0</v>
+        <v>6579952.0</v>
       </c>
       <c r="E4" t="n">
-        <v>76672.0</v>
+        <v>1.341709E7</v>
       </c>
       <c r="F4" t="n">
-        <v>119537.0</v>
+        <v>2.1487025E7</v>
       </c>
       <c r="G4" t="n">
-        <v>186550.0</v>
+        <v>2.8006605E7</v>
       </c>
       <c r="H4" t="n">
-        <v>220962.0</v>
+        <v>4.0900873E7</v>
       </c>
       <c r="I4" t="n">
-        <v>319369.0</v>
+        <v>5.2917933E7</v>
       </c>
       <c r="J4" t="n">
-        <v>356799.0</v>
+        <v>6.7700035E7</v>
       </c>
       <c r="K4" t="n">
-        <v>517993.0</v>
+        <v>8.0648034E7</v>
       </c>
       <c r="L4" t="n">
-        <v>511351.0</v>
+        <v>9.9562E7</v>
       </c>
       <c r="M4" t="n">
-        <v>648396.0</v>
+        <v>1.20064357E8</v>
       </c>
       <c r="N4" t="n">
-        <v>784838.0</v>
+        <v>1.31465019E8</v>
       </c>
       <c r="O4" t="n">
-        <v>660471.0</v>
+        <v>1.6640113E8</v>
       </c>
       <c r="P4" t="n">
-        <v>933956.0</v>
+        <v>1.85073005E8</v>
       </c>
     </row>
     <row r="5">
@@ -3793,49 +3793,49 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>22941.0</v>
+        <v>212510.0</v>
       </c>
       <c r="C5" t="n">
-        <v>41053.0</v>
+        <v>268052.0</v>
       </c>
       <c r="D5" t="n">
-        <v>61579.0</v>
+        <v>497465.0</v>
       </c>
       <c r="E5" t="n">
-        <v>83313.0</v>
+        <v>554819.0</v>
       </c>
       <c r="F5" t="n">
-        <v>103237.0</v>
+        <v>1173030.0</v>
       </c>
       <c r="G5" t="n">
-        <v>121952.0</v>
+        <v>854869.0</v>
       </c>
       <c r="H5" t="n">
-        <v>154552.0</v>
+        <v>1235213.0</v>
       </c>
       <c r="I5" t="n">
-        <v>165420.0</v>
+        <v>1391577.0</v>
       </c>
       <c r="J5" t="n">
-        <v>188361.0</v>
+        <v>1389765.0</v>
       </c>
       <c r="K5" t="n">
-        <v>222773.0</v>
+        <v>1837726.0</v>
       </c>
       <c r="L5" t="n">
-        <v>263826.0</v>
+        <v>1688607.0</v>
       </c>
       <c r="M5" t="n">
-        <v>256581.0</v>
+        <v>2098533.0</v>
       </c>
       <c r="N5" t="n">
-        <v>275297.0</v>
+        <v>2631619.0</v>
       </c>
       <c r="O5" t="n">
-        <v>207680.0</v>
+        <v>3528748.0</v>
       </c>
       <c r="P5" t="n">
-        <v>323595.0</v>
+        <v>3292693.0</v>
       </c>
     </row>
     <row r="6">
@@ -3843,49 +3843,49 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>4226.0</v>
+        <v>12075.0</v>
       </c>
       <c r="C6" t="n">
-        <v>7848.0</v>
+        <v>13886.0</v>
       </c>
       <c r="D6" t="n">
-        <v>15093.0</v>
+        <v>16301.0</v>
       </c>
       <c r="E6" t="n">
-        <v>16301.0</v>
+        <v>20527.0</v>
       </c>
       <c r="F6" t="n">
-        <v>18716.0</v>
+        <v>37431.0</v>
       </c>
       <c r="G6" t="n">
-        <v>21131.0</v>
+        <v>27167.0</v>
       </c>
       <c r="H6" t="n">
-        <v>24148.0</v>
+        <v>31997.0</v>
       </c>
       <c r="I6" t="n">
-        <v>50712.0</v>
+        <v>35619.0</v>
       </c>
       <c r="J6" t="n">
-        <v>28375.0</v>
+        <v>36223.0</v>
       </c>
       <c r="K6" t="n">
-        <v>30790.0</v>
+        <v>43468.0</v>
       </c>
       <c r="L6" t="n">
-        <v>156968.0</v>
+        <v>58561.0</v>
       </c>
       <c r="M6" t="n">
-        <v>36827.0</v>
+        <v>50713.0</v>
       </c>
       <c r="N6" t="n">
-        <v>55542.0</v>
+        <v>51316.0</v>
       </c>
       <c r="O6" t="n">
-        <v>46486.0</v>
+        <v>63995.0</v>
       </c>
       <c r="P6" t="n">
-        <v>43468.0</v>
+        <v>82709.0</v>
       </c>
     </row>
   </sheetData>
@@ -3910,49 +3910,49 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>100.0</v>
+        <v>1000.0</v>
       </c>
       <c r="C1" t="n">
-        <v>200.0</v>
+        <v>2000.0</v>
       </c>
       <c r="D1" t="n">
-        <v>300.0</v>
+        <v>3000.0</v>
       </c>
       <c r="E1" t="n">
-        <v>400.0</v>
+        <v>4000.0</v>
       </c>
       <c r="F1" t="n">
-        <v>500.0</v>
+        <v>5000.0</v>
       </c>
       <c r="G1" t="n">
-        <v>600.0</v>
+        <v>6000.0</v>
       </c>
       <c r="H1" t="n">
-        <v>700.0</v>
+        <v>7000.0</v>
       </c>
       <c r="I1" t="n">
-        <v>800.0</v>
+        <v>8000.0</v>
       </c>
       <c r="J1" t="n">
-        <v>900.0</v>
+        <v>9000.0</v>
       </c>
       <c r="K1" t="n">
-        <v>1000.0</v>
+        <v>10000.0</v>
       </c>
       <c r="L1" t="n">
-        <v>1100.0</v>
+        <v>11000.0</v>
       </c>
       <c r="M1" t="n">
-        <v>1200.0</v>
+        <v>12000.0</v>
       </c>
       <c r="N1" t="n">
-        <v>1300.0</v>
+        <v>13000.0</v>
       </c>
       <c r="O1" t="n">
-        <v>1400.0</v>
+        <v>14000.0</v>
       </c>
       <c r="P1" t="n">
-        <v>1500.0</v>
+        <v>15000.0</v>
       </c>
     </row>
     <row r="2">
@@ -3960,49 +3960,49 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>13282.0</v>
+        <v>1939151.0</v>
       </c>
       <c r="C2" t="n">
-        <v>53128.0</v>
+        <v>6902943.0</v>
       </c>
       <c r="D2" t="n">
-        <v>91766.0</v>
+        <v>1.2691417E7</v>
       </c>
       <c r="E2" t="n">
-        <v>1489984.0</v>
+        <v>2.4389714E7</v>
       </c>
       <c r="F2" t="n">
-        <v>543952.0</v>
+        <v>4.0407633E7</v>
       </c>
       <c r="G2" t="n">
-        <v>1313093.0</v>
+        <v>6.1989441E7</v>
       </c>
       <c r="H2" t="n">
-        <v>489014.0</v>
+        <v>9.0489285E7</v>
       </c>
       <c r="I2" t="n">
-        <v>650207.0</v>
+        <v>1.20439871E8</v>
       </c>
       <c r="J2" t="n">
-        <v>1333016.0</v>
+        <v>1.4930557E8</v>
       </c>
       <c r="K2" t="n">
-        <v>1259362.0</v>
+        <v>2.27620223E8</v>
       </c>
       <c r="L2" t="n">
-        <v>1221328.0</v>
+        <v>2.41519082E8</v>
       </c>
       <c r="M2" t="n">
-        <v>1327582.0</v>
+        <v>2.92253961E8</v>
       </c>
       <c r="N2" t="n">
-        <v>1520773.0</v>
+        <v>3.54339393E8</v>
       </c>
       <c r="O2" t="n">
-        <v>1647555.0</v>
+        <v>5.13628694E8</v>
       </c>
       <c r="P2" t="n">
-        <v>1239439.0</v>
+        <v>6.43312737E8</v>
       </c>
     </row>
     <row r="3">
@@ -4010,49 +4010,49 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>24752.0</v>
+        <v>600702.0</v>
       </c>
       <c r="C3" t="n">
-        <v>159382.0</v>
+        <v>4129450.0</v>
       </c>
       <c r="D3" t="n">
-        <v>200436.0</v>
+        <v>4979489.0</v>
       </c>
       <c r="E3" t="n">
-        <v>301257.0</v>
+        <v>1.3048216E7</v>
       </c>
       <c r="F3" t="n">
-        <v>453998.0</v>
+        <v>1.482557E7</v>
       </c>
       <c r="G3" t="n">
-        <v>2394357.0</v>
+        <v>1.9929425E7</v>
       </c>
       <c r="H3" t="n">
-        <v>955690.0</v>
+        <v>2.7543551E7</v>
       </c>
       <c r="I3" t="n">
-        <v>1255740.0</v>
+        <v>3.9020282E7</v>
       </c>
       <c r="J3" t="n">
-        <v>1452553.0</v>
+        <v>4.4323365E7</v>
       </c>
       <c r="K3" t="n">
-        <v>2.059836E7</v>
+        <v>5.5433034E7</v>
       </c>
       <c r="L3" t="n">
-        <v>7913576.0</v>
+        <v>7.11829E7</v>
       </c>
       <c r="M3" t="n">
-        <v>2404018.0</v>
+        <v>7.3801237E7</v>
       </c>
       <c r="N3" t="n">
-        <v>3621723.0</v>
+        <v>1.05738064E8</v>
       </c>
       <c r="O3" t="n">
-        <v>3109163.0</v>
+        <v>1.12300508E8</v>
       </c>
       <c r="P3" t="n">
-        <v>5793308.0</v>
+        <v>1.73700114E8</v>
       </c>
     </row>
     <row r="4">
@@ -4060,49 +4060,49 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>14490.0</v>
+        <v>1805729.0</v>
       </c>
       <c r="C4" t="n">
-        <v>172664.0</v>
+        <v>5299461.0</v>
       </c>
       <c r="D4" t="n">
-        <v>95991.0</v>
+        <v>1.1910202E7</v>
       </c>
       <c r="E4" t="n">
-        <v>143685.0</v>
+        <v>2.4334171E7</v>
       </c>
       <c r="F4" t="n">
-        <v>542142.0</v>
+        <v>4.0091283E7</v>
       </c>
       <c r="G4" t="n">
-        <v>321180.0</v>
+        <v>5.9855289E7</v>
       </c>
       <c r="H4" t="n">
-        <v>485392.0</v>
+        <v>8.059551E7</v>
       </c>
       <c r="I4" t="n">
-        <v>557235.0</v>
+        <v>1.12750883E8</v>
       </c>
       <c r="J4" t="n">
-        <v>773971.0</v>
+        <v>1.47025921E8</v>
       </c>
       <c r="K4" t="n">
-        <v>957502.0</v>
+        <v>1.83634338E8</v>
       </c>
       <c r="L4" t="n">
-        <v>1063152.0</v>
+        <v>2.7331162E8</v>
       </c>
       <c r="M4" t="n">
-        <v>1222535.0</v>
+        <v>2.90265909E8</v>
       </c>
       <c r="N4" t="n">
-        <v>1301623.0</v>
+        <v>3.43838275E8</v>
       </c>
       <c r="O4" t="n">
-        <v>1191141.0</v>
+        <v>3.9375632E8</v>
       </c>
       <c r="P4" t="n">
-        <v>3051810.0</v>
+        <v>5.59637044E8</v>
       </c>
     </row>
     <row r="5">
@@ -4110,49 +4110,49 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>21130.0</v>
+        <v>281333.0</v>
       </c>
       <c r="C5" t="n">
-        <v>44675.0</v>
+        <v>342913.0</v>
       </c>
       <c r="D5" t="n">
-        <v>95388.0</v>
+        <v>549385.0</v>
       </c>
       <c r="E5" t="n">
-        <v>84521.0</v>
+        <v>554820.0</v>
       </c>
       <c r="F5" t="n">
-        <v>109877.0</v>
+        <v>649604.0</v>
       </c>
       <c r="G5" t="n">
-        <v>145496.0</v>
+        <v>728087.0</v>
       </c>
       <c r="H5" t="n">
-        <v>193795.0</v>
+        <v>898337.0</v>
       </c>
       <c r="I5" t="n">
-        <v>185946.0</v>
+        <v>1427800.0</v>
       </c>
       <c r="J5" t="n">
-        <v>202851.0</v>
+        <v>1214686.0</v>
       </c>
       <c r="K5" t="n">
-        <v>204662.0</v>
+        <v>1237023.0</v>
       </c>
       <c r="L5" t="n">
-        <v>245111.0</v>
+        <v>1778561.0</v>
       </c>
       <c r="M5" t="n">
-        <v>268052.0</v>
+        <v>1738716.0</v>
       </c>
       <c r="N5" t="n">
-        <v>285560.0</v>
+        <v>1832896.0</v>
       </c>
       <c r="O5" t="n">
-        <v>237866.0</v>
+        <v>1942774.0</v>
       </c>
       <c r="P5" t="n">
-        <v>353781.0</v>
+        <v>2448691.0</v>
       </c>
     </row>
     <row r="6">
@@ -4160,49 +4160,49 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>13885.0</v>
+        <v>51316.0</v>
       </c>
       <c r="C6" t="n">
-        <v>10867.0</v>
+        <v>56750.0</v>
       </c>
       <c r="D6" t="n">
-        <v>19319.0</v>
+        <v>78484.0</v>
       </c>
       <c r="E6" t="n">
-        <v>205869.0</v>
+        <v>93576.0</v>
       </c>
       <c r="F6" t="n">
-        <v>24149.0</v>
+        <v>115311.0</v>
       </c>
       <c r="G6" t="n">
-        <v>96595.0</v>
+        <v>120141.0</v>
       </c>
       <c r="H6" t="n">
-        <v>27772.0</v>
+        <v>148516.0</v>
       </c>
       <c r="I6" t="n">
-        <v>29582.0</v>
+        <v>167834.0</v>
       </c>
       <c r="J6" t="n">
-        <v>36224.0</v>
+        <v>223981.0</v>
       </c>
       <c r="K6" t="n">
-        <v>38034.0</v>
+        <v>184739.0</v>
       </c>
       <c r="L6" t="n">
-        <v>18112.0</v>
+        <v>194398.0</v>
       </c>
       <c r="M6" t="n">
-        <v>17508.0</v>
+        <v>228207.0</v>
       </c>
       <c r="N6" t="n">
-        <v>16904.0</v>
+        <v>272278.0</v>
       </c>
       <c r="O6" t="n">
-        <v>13282.0</v>
+        <v>251148.0</v>
       </c>
       <c r="P6" t="n">
-        <v>19922.0</v>
+        <v>298841.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>